<commit_message>
Deploying to gh-pages from @ vojtapolasek/content@d44911404319a99b77eaba443d108b6e514c7778 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -642,7 +642,7 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>The operating system must manage excess capacity, bandwidth, or other redundancy to limit the effects of information flooding types of Denial of Service (DoS) attacks.</t>
+          <t>Red Hat Enterprise Linux 9 must manage excess capacity, bandwidth, or other redundancy to limit the effects of information flooding types of Denial of Service (DoS) attacks.</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
@@ -695,7 +695,15 @@
         </is>
       </c>
       <c r="L3" s="2" t="n"/>
-      <c r="M3" s="2" t="inlineStr"/>
+      <c r="M3" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to use TCP syncookies.
+Add or edit the following line in a system configuration file in the "/etc/sysctl.d/" directory:
+ net.ipv4.tcp_syncookies = 1
+ Load settings from all system configuration files with the following command:
+ $ sudo sysctl --system</t>
+        </is>
+      </c>
       <c r="N3" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -3945,7 +3953,7 @@
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require individuals to be authenticated with an individual authenticator prior to using a group authenticator.</t>
+          <t>Red Hat Enterprise Linux 9must require individuals to be authenticated with an individual authenticator prior to using a group authenticator.</t>
         </is>
       </c>
       <c r="G50" s="2" t="inlineStr">
@@ -4999,7 +5007,7 @@
       </c>
       <c r="F65" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for network access to non-privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for network access to non-privileged accounts.</t>
         </is>
       </c>
       <c r="G65" s="2" t="inlineStr">
@@ -6042,7 +6050,7 @@
       </c>
       <c r="F80" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for local access to privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for local access to privileged accounts.</t>
         </is>
       </c>
       <c r="G80" s="2" t="inlineStr">
@@ -6088,7 +6096,14 @@
         </is>
       </c>
       <c r="L80" s="2" t="n"/>
-      <c r="M80" s="2" t="inlineStr"/>
+      <c r="M80" s="2" t="inlineStr">
+        <is>
+          <t>To configure the system add or modify the following line in "/etc/ssh/sshd_config".
+PubkeyAuthentication yes
+Restart the SSH daemon for the settings to take effect:
+$ sudo systemctl restart sshd.service</t>
+        </is>
+      </c>
       <c r="N80" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -9410,7 +9425,7 @@
       </c>
       <c r="F129" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for local access to non-privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for local access to non-privileged accounts.</t>
         </is>
       </c>
       <c r="G129" s="2" t="inlineStr">
@@ -10979,7 +10994,7 @@
       </c>
       <c r="F151" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use multifactor authentication for network access to privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 must use multifactor authentication for network access to privileged accounts.</t>
         </is>
       </c>
       <c r="G151" s="2" t="inlineStr">
@@ -12813,7 +12828,7 @@
       </c>
       <c r="F181" s="2" t="inlineStr">
         <is>
-          <t>The operating system must isolate security functions from nonsecurity functions.</t>
+          <t>Red Hat Enterprise Linux 9 must isolate security functions from nonsecurity functions.</t>
         </is>
       </c>
       <c r="G181" s="2" t="inlineStr">
@@ -12857,7 +12872,16 @@
         </is>
       </c>
       <c r="L181" s="2" t="n"/>
-      <c r="M181" s="2" t="inlineStr"/>
+      <c r="M181" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To ensure that "vsyscall=none" is added as a kernel command line
+argument to newly installed kernels, add "vsyscall=none" to the
+default Grub2 command line for Linux operating systems.  Modify the line within
+"/etc/default/grub" as shown below:
+ GRUB_CMDLINE_LINUX="... vsyscall=none ..." 
+Run the following command to update command line for already installed kernels: # grubby --update-kernel=ALL --args="vsyscall=none" </t>
+        </is>
+      </c>
       <c r="N181" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ vojtapolasek/content@6602cecc7ce21c62273010f990712f3952d1b275 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -7505,7 +7505,7 @@
       </c>
       <c r="F100" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow the use of a temporary password for system logons with an immediate change to a permanent password.</t>
+          <t>Red Hat Enterprise Linux 9 must allow the use of a temporary password for system logons with an immediate change to a permanent password.</t>
         </is>
       </c>
       <c r="G100" s="2" t="inlineStr">
@@ -7514,10 +7514,17 @@
 Temporary passwords are typically used to allow access when new accounts are created or passwords are changed. It is common practice for administrators to create temporary passwords for user accounts which allow the users to log on, yet force them to change the password once they have successfully authenticated.</t>
         </is>
       </c>
-      <c r="H100" s="2" t="inlineStr"/>
+      <c r="H100" s="2" t="inlineStr">
+        <is>
+          <t>Without providing this capability, an account may be created without a password.
+Non-repudiation cannot be guaranteed once an account is created if a user is not forced to change the temporary password upon initial logon.
+Temporary passwords are typically used to allow access when new accounts are created or passwords are changed.
+It is common practice for administrators to create temporary passwords for user accounts that allow the users to log on, yet force them to change the password once they have successfully authenticated.</t>
+        </is>
+      </c>
       <c r="I100" s="2" t="inlineStr">
         <is>
-          <t>Applicable - Configurable</t>
+          <t>Applicable - Inherently Met</t>
         </is>
       </c>
       <c r="J100" s="2" t="inlineStr">
@@ -7525,7 +7532,12 @@
           <t>Verify the operating system allows the use of a temporary password for system logons with an immediate change to a permanent password. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K100" s="2" t="n"/>
+      <c r="K100" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 supports this requirement and cannot be configured to be out of compliance.
+Red Hat Enterprise Linux 9 inherently meets this requirement.</t>
+        </is>
+      </c>
       <c r="L100" s="2" t="n"/>
       <c r="M100" s="2" t="n"/>
       <c r="N100" s="2" t="inlineStr">
@@ -7534,8 +7546,21 @@
         </is>
       </c>
       <c r="O100" s="2" t="n"/>
-      <c r="P100" s="2" t="n"/>
-      <c r="Q100" s="2" t="n"/>
+      <c r="P100" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 offers the following commands to facilitate the use of a temporary password.
+chage -d 0 [username]
+(forces the user to change their password at next logon)
+passwd -e [username]
+(expires the passwd for a given user forcing a change at next logon.)</t>
+        </is>
+      </c>
+      <c r="Q100" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 has the capability to perform temporary passwords based on organization policy.
+Configuration is not appropriate to define at an enterprise level.</t>
+        </is>
+      </c>
     </row>
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
@@ -7701,7 +7726,7 @@
       </c>
       <c r="F103" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement replay-resistant authentication mechanisms for network access to non-privileged accounts.</t>
+          <t>Red Hat Enterprise Linux 9 system must implement replay-resistant authentication mechanisms for network access to non-privileged accounts.</t>
         </is>
       </c>
       <c r="G103" s="2" t="inlineStr">
@@ -7715,7 +7740,7 @@
       <c r="H103" s="2" t="inlineStr"/>
       <c r="I103" s="2" t="inlineStr">
         <is>
-          <t>Applicable - Configurable</t>
+          <t>Applicable - Inherently Met</t>
         </is>
       </c>
       <c r="J103" s="2" t="inlineStr">
@@ -7723,17 +7748,36 @@
           <t>Verify the operating system implements replay-resistant authentication mechanisms for network access to non-privileged accounts. If it does not, this is a finding.</t>
         </is>
       </c>
-      <c r="K103" s="2" t="n"/>
+      <c r="K103" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 supports this requirement and cannot be configured to be out of compliance.
+Red Hat Enterprise Linux 9 inherently meets this requirement.</t>
+        </is>
+      </c>
       <c r="L103" s="2" t="n"/>
-      <c r="M103" s="2" t="n"/>
+      <c r="M103" s="2" t="inlineStr">
+        <is>
+          <t>Red Hat Enterprise Linux 9 inherently meets this requirement.
+No fix is required.</t>
+        </is>
+      </c>
       <c r="N103" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
         </is>
       </c>
       <c r="O103" s="2" t="n"/>
-      <c r="P103" s="2" t="n"/>
-      <c r="Q103" s="2" t="n"/>
+      <c r="P103" s="2" t="inlineStr">
+        <is>
+          <t>The release notes of OpenSSH 7.6 states "OpenSSH is a 100% complete SSH protocol 2.0 implementation and includes sftp client and server support."
+https://www.openssh.com/txt/release-7.6</t>
+        </is>
+      </c>
+      <c r="Q103" s="2" t="inlineStr">
+        <is>
+          <t>The OpenSSH package in Red Hat Enterprise Linux 9 is version 8.7, which is newer than 7.6 which only supports SSH protocol 2.0 which is restraint to replay attacks.</t>
+        </is>
+      </c>
     </row>
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ vojtapolasek/content@b4ede572458fc0a3e3ca8f984e777ee7c2bf2ef6 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4, AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -621,7 +621,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, SC-5, SC-5 (2)</t>
+          <t>SC-5 (2),SC-5,CM-6 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -716,7 +716,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (8), AC-6 (9), AU-12 (3), AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 b, AU-7 b, AU-8 b, AU-8 b, CM-5 (1)</t>
+          <t>AU-7 b,AU-12 (3),AU-8 b,CM-5 (1),AC-6 (9),AC-6 (8),AU-7 a</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -792,7 +792,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b, AC-17 (1), AC-17 (9), CM-6 b, CM-6 b</t>
+          <t>AC-17 (9),CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1008,7 +1008,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11), IA-2 (12)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1155,7 +1155,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b), CM-7 (2)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1307,7 +1307,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b, AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>IA-2, IA-8, AU-3 (1)</t>
+          <t>AU-3 (1),IA-8,IA-2</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1596,7 +1596,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10), CM-6 b</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1668,7 +1668,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b), IA-5 (1) (a), IA-5 (1) (a), IA-5 (1) (a), IA-5 (1) (a), CM-6 b, IA-5 (1) (a)</t>
+          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1943,7 +1943,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e, SC-10, AC-12, MA-4 (7)</t>
+          <t>MA-4 (7),SC-10,MA-4 e,AC-12</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2014,7 +2014,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3, AU-3, AU-3, AU-3, AU-3 (1), AU-6 (4), AU-7 (1), AU-7 a, AU-14 (1), AU-3, CM-5 (1), MA-4 (1) (a), CM-6 b, AU-12 a, AU-7 a</t>
+          <t>AU-3,AU-14 (1),AU-12 a,AU-7 (1),CM-6 b,CM-5 (1),AU-6 (4),AU-3 (1),MA-4 (1) (a),AU-7 a</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2243,7 +2243,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2509,7 +2509,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8, SC-8 (1), SC-8 (2), SC-8 (2)</t>
+          <t>SC-8 (2),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2634,7 +2634,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4), AU-3, AU-3 (1), AU-12 a, AC-2 (4), MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AU-12 c, AU-12 c</t>
+          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -2838,7 +2838,7 @@
     <row r="34" ht="130" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a, AC-11 b</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -3110,7 +3110,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9, SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3178,7 +3178,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AU-3, CM-6 b</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3305,7 +3305,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1), AU-4 (1)</t>
+          <t>AU-4 (1)</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3377,7 +3377,7 @@
     <row r="42" ht="130" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1), SC-28, SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
@@ -3439,7 +3439,13 @@
         </is>
       </c>
       <c r="L42" s="2" t="n"/>
-      <c r="M42" s="2" t="inlineStr"/>
+      <c r="M42" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to prevent unauthorized modification of all information at rest by using disk encryption.
+Encrypting a partition in an already installed system is more difficult, because existing partitions will need to be resized and changed.
+To encrypt an entire partition, dedicate a partition for encryption in the partition layout.</t>
+        </is>
+      </c>
       <c r="N42" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -3523,7 +3529,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>IA-11, IA-11, IA-11</t>
+          <t>IA-11</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -3593,7 +3599,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a, AC-8 b, AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 b,AC-8 a</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3804,7 +3810,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, CM-6 b</t>
+          <t>CM-6 b</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -3932,7 +3938,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5), CM-6 b</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4140,7 +4146,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>SC-13, MA-4 (6), MA-4 (6)</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4277,7 +4283,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2), SC-8</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4348,7 +4354,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a), AU-12 c, AU-12 c</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4835,7 +4841,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a, AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -4986,7 +4992,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2), CM-6 b, CM-6 b</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5126,7 +5132,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5252,7 +5258,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-7 a, AU-12 (3), AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 a, AU-7 b, AU-7 b, AU-8 b, AU-8 b, CM-5 (1), AU-12 c, AU-12 c, CM-6 b, AU-12 a</t>
+          <t>AU-7 b,AU-12 (3),AU-12 a,AU-12 c,AU-8 b,CM-6 b,CM-5 (1),AU-7 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5402,7 +5408,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-4 (1), AU-4 (1)</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5793,7 +5799,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4), AU-3, AU-3 (1), AU-12 a, AC-2 (4), MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AU-12 c, AU-12 c, AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4)</t>
+          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -5958,7 +5964,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9, AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6029,7 +6035,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1), IA-2 (2), IA-2 (3), IA-2 (4)</t>
+          <t>IA-2 (1),IA-2 (4),IA-2 (2),IA-2 (3)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6116,7 +6122,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, CM-5 (3)</t>
+          <t>CM-5 (3),CM-6 b</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6449,7 +6455,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6595,7 +6601,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4), AC-2 (4), AC-2 (4), AC-2 (4), AU-12 c, AC-6 (9), AU-12 c, CM-5 (1), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>CM-5 (1),AC-2 (4),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6662,7 +6668,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2, IA-2 (2), IA-2 (3), IA-2 (5), IA-2 (4)</t>
+          <t>IA-2 (4),IA-2 (5),IA-2 (2),IA-2 (3),IA-2</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6742,7 +6748,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11), IA-2 (12)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -6818,7 +6824,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7192,7 +7198,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1), AC-18 (1), SC-8 (1), SC-8</t>
+          <t>AC-18 (1),SC-8 (1),SC-8</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7268,7 +7274,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (a), AU-8 (1) (b), AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7416,7 +7422,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-9, AU-9, AU-9</t>
+          <t>AU-9</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -7565,7 +7571,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>IA-11, AC-3 (4)</t>
+          <t>IA-11,AC-3 (4)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -7635,7 +7641,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8221,7 +8227,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a, AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -8763,7 +8769,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9053,7 +9059,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>CM-7 b, CM-7 a</t>
+          <t>CM-7 b,CM-7 a</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -9123,7 +9129,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9193,7 +9199,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>CM-7 a, AC-18 (1)</t>
+          <t>AC-18 (1),CM-7 a</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -9378,7 +9384,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c), CM-7 a, CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -9940,7 +9946,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1), AC-11 b</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10161,7 +10167,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>CM-3 (5), SI-6 b, SI-6 d</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -10354,7 +10360,7 @@
     <row r="142" ht="130" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (2), AC-2 (2)</t>
+          <t>AC-2 (2)</t>
         </is>
       </c>
       <c r="B142" s="2" t="inlineStr">
@@ -10803,7 +10809,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-14 (1)</t>
+          <t>AU-3,AU-14 (1),AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11364,7 +11370,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-3, AU-3 (1), AU-12 a, MA-4 (1) (a), AU-12 c, AU-12 c, AU-12 c, AU-12 c, AU-12 c</t>
+          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11496,7 +11502,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>SC-8, AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -12479,7 +12485,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>SI-16, CM-7 a</t>
+          <t>SI-16,CM-7 a</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -12851,7 +12857,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b, SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -13673,7 +13679,7 @@
       </c>
       <c r="F192" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect the confidentiality and integrity of all information at rest.</t>
+          <t>Red Hat Enterprise Linux 9 must protect the confidentiality and integrity of all information at rest.</t>
         </is>
       </c>
       <c r="G192" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ vojtapolasek/content@e732c1ecc2c95634f4fbfa0e13dffc08a5de7b9b 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -554,7 +554,11 @@
           <t>SRG-OS-000341-GPOS-00132,SRG-OS-000342-GPOS-00133</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr"/>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88173-0</t>
+        </is>
+      </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
           <t>The operating system must allocate audit record storage capacity to store at least one weeks worth of audit records, when audit records are not immediately sent to a central audit record storage facility.</t>
@@ -562,7 +566,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allocate audit record storage capacity to store at least one weeks worth of audit records, when audit records are not immediately sent to a central audit record storage facility.</t>
+          <t>Red Hat Enterprise Linux 9 must allocate audit record storage capacity to store at least one weeks worth of audit records, when audit records are not immediately sent to a central audit record storage facility.</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
@@ -621,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),SC-5,CM-6 b</t>
+          <t>SC-5,CM-6 b,SC-5 (2)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -634,7 +638,11 @@
           <t>SRG-OS-000480-GPOS-00227,SRG-OS-000420-GPOS-00186,SRG-OS-000142-GPOS-00071</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr"/>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84006-6</t>
+        </is>
+      </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
           <t>The operating system must manage excess capacity, bandwidth, or other redundancy to limit the effects of information flooding types of Denial of Service (DoS) attacks.</t>
@@ -716,7 +724,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-12 (3),AU-8 b,CM-5 (1),AC-6 (9),AC-6 (8),AU-7 a</t>
+          <t>AU-12 (3),AC-6 (8),CM-5 (1),AU-8 b,AC-6 (9),AU-7 a,AU-7 b</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -729,7 +737,11 @@
           <t>SRG-OS-000326-GPOS-00126,SRG-OS-000327-GPOS-00127,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000359-GPOS-00146,SRG-OS-000365-GPOS-00152</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr"/>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86402-5</t>
+        </is>
+      </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide a report generation capability that supports on-demand audit review and analysis.</t>
@@ -737,7 +749,7 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide a report generation capability that supports on-demand audit review and analysis.</t>
+          <t>Red Hat Enterprise Linux 9 must provide a report generation capability that supports on-demand audit review and analysis.</t>
         </is>
       </c>
       <c r="G4" s="2" t="inlineStr">
@@ -792,7 +804,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (9),CM-7 b,AC-17 (1),CM-6 b</t>
+          <t>AC-17 (1),AC-17 (9),CM-6 b,CM-7 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -805,7 +817,11 @@
           <t>SRG-OS-000096-GPOS-00050,SRG-OS-000297-GPOS-00115,SRG-OS-000298-GPOS-00116,SRG-OS-000480-GPOS-00227,SRG-OS-000480-GPOS-00232</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr"/>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84021-5</t>
+        </is>
+      </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide the capability to immediately disconnect or disable remote access to the operating system.</t>
@@ -813,7 +829,7 @@
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide the capability to immediately disconnect or disable remote access to the operating system.</t>
+          <t>Red Hat Enterprise Linux 9 must provide the capability to immediately disconnect or disable remote access to the operating system.</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
@@ -973,7 +989,7 @@
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require devices to re-authenticate when changing authenticators.</t>
+          <t>Red Hat Enterprise Linux 9 must require devices to re-authenticate when changing authenticators.</t>
         </is>
       </c>
       <c r="G7" s="2" t="inlineStr">
@@ -1008,7 +1024,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1021,7 +1037,11 @@
           <t>SRG-OS-000375-GPOS-00160,SRG-OS-000376-GPOS-00161</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr"/>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83595-9</t>
+        </is>
+      </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
           <t>The operating system must accept Personal Identity Verification (PIV) credentials.</t>
@@ -1029,7 +1049,7 @@
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>The operating system must accept Personal Identity Verification (PIV) credentials.</t>
+          <t>Red Hat Enterprise Linux 9 must accept Personal Identity Verification (PIV) credentials.</t>
         </is>
       </c>
       <c r="G8" s="2" t="inlineStr">
@@ -1155,7 +1175,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1168,7 +1188,11 @@
           <t>SRG-OS-000370-GPOS-00155,SRG-OS-000368-GPOS-00154</t>
         </is>
       </c>
-      <c r="D10" s="2" t="inlineStr"/>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84224-5</t>
+        </is>
+      </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
           <t>The operating system must prevent program execution in accordance with local policies regarding software program usage and restrictions and/or rules authorizing the terms and conditions of software program usage.</t>
@@ -1176,7 +1200,7 @@
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent program execution in accordance with local policies regarding software program usage and restrictions and/or rules authorizing the terms and conditions of software program usage.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent program execution in accordance with local policies regarding software program usage and restrictions and/or rules authorizing the terms and conditions of software program usage.</t>
         </is>
       </c>
       <c r="G10" s="2" t="inlineStr">
@@ -1240,7 +1264,11 @@
           <t>SRG-OS-000118-GPOS-00060</t>
         </is>
       </c>
-      <c r="D11" s="2" t="inlineStr"/>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83627-0</t>
+        </is>
+      </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
           <t>The operating system must disable account identifiers (individuals, groups, roles, and devices) after 35 days of inactivity.</t>
@@ -1307,7 +1335,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>AC-7 a,AC-7 b</t>
+          <t>AC-7 b,AC-7 a</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1320,7 +1348,11 @@
           <t>SRG-OS-000329-GPOS-00128,SRG-OS-000021-GPOS-00005</t>
         </is>
       </c>
-      <c r="D12" s="2" t="inlineStr"/>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83587-6</t>
+        </is>
+      </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce the limit of three consecutive invalid logon attempts by a user during a 15-minute time period.</t>
@@ -1328,7 +1360,7 @@
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce the limit of three consecutive invalid logon attempts by a user during a 15-minute time period.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce the limit of three consecutive invalid logon attempts by a user during a 15-minute time period.</t>
         </is>
       </c>
       <c r="G12" s="2" t="inlineStr">
@@ -1400,7 +1432,11 @@
           <t>SRG-OS-000076-GPOS-00044</t>
         </is>
       </c>
-      <c r="D13" s="2" t="inlineStr"/>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83606-4</t>
+        </is>
+      </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
           <t>Operating systems must enforce a 60-day maximum password lifetime restriction.</t>
@@ -1487,7 +1523,7 @@
       </c>
       <c r="F14" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow operating system admins to pass information to any other operating system admin or user.</t>
+          <t>Red Hat Enterprise Linux 9 must allow operating system admins to pass information to any other operating system admin or user.</t>
         </is>
       </c>
       <c r="G14" s="2" t="inlineStr">
@@ -1535,7 +1571,11 @@
           <t>SRG-OS-000104-GPOS-00051,SRG-OS-000121-GPOS-00062,SRG-OS-000042-GPOS-00020</t>
         </is>
       </c>
-      <c r="D15" s="2" t="inlineStr"/>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88493-2</t>
+        </is>
+      </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records containing the full-text recording of privileged commands.</t>
@@ -1543,7 +1583,7 @@
       </c>
       <c r="F15" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records containing the full-text recording of privileged commands.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records containing the full-text recording of privileged commands.</t>
         </is>
       </c>
       <c r="G15" s="2" t="inlineStr">
@@ -1596,7 +1636,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (10),CM-6 b</t>
+          <t>CM-6 b,AC-6 (10)</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1609,7 +1649,11 @@
           <t>SRG-OS-000324-GPOS-00125,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D16" s="2" t="inlineStr"/>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90308-8</t>
+        </is>
+      </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
           <t>The operating system must prevent non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.</t>
@@ -1617,7 +1661,7 @@
       </c>
       <c r="F16" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.</t>
         </is>
       </c>
       <c r="G16" s="2" t="inlineStr">
@@ -1668,7 +1712,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1681,7 +1725,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000064-GPOS-00033,SRG-OS-000466-GPOS-00210,SRG-OS-000458-GPOS-00203</t>
         </is>
       </c>
-      <c r="D17" s="2" t="inlineStr"/>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83830-0</t>
+        </is>
+      </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to modify privileges occur.</t>
@@ -1689,7 +1737,7 @@
       </c>
       <c r="F17" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to modify privileges occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to modify privileges occur.</t>
         </is>
       </c>
       <c r="G17" s="2" t="inlineStr">
@@ -1760,7 +1808,7 @@
       </c>
       <c r="F18" s="2" t="inlineStr">
         <is>
-          <t>In the event of a system failure, the operating system must preserve any information necessary to determine cause of failure and any information necessary to return to operations with least disruption to mission processes.</t>
+          <t>In the event of a system failure, Red Hat Enterprise Linux 9 must preserve any information necessary to determine cause of failure and any information necessary to return to operations with least disruption to mission processes.</t>
         </is>
       </c>
       <c r="G18" s="2" t="inlineStr">
@@ -1795,7 +1843,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),IA-5 (1) (b),CM-6 b</t>
+          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1808,7 +1856,11 @@
           <t>SRG-OS-000072-GPOS-00040,SRG-OS-000071-GPOS-00039,SRG-OS-000070-GPOS-00038,SRG-OS-000266-GPOS-00101,SRG-OS-000078-GPOS-00046,SRG-OS-000480-GPOS-00225,SRG-OS-000069-GPOS-00037</t>
         </is>
       </c>
-      <c r="D19" s="2" t="inlineStr"/>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86356-3</t>
+        </is>
+      </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce password complexity by requiring that at least one lower-case character be used.</t>
@@ -1886,7 +1938,11 @@
           <t>SRG-OS-000478-GPOS-00223</t>
         </is>
       </c>
-      <c r="D20" s="2" t="inlineStr"/>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86547-7</t>
+        </is>
+      </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement NIST FIPS-validated cryptography for the following: to provision digital signatures, to generate cryptographic hashes, and to protect unclassified information requiring confidentiality and cryptographic protection in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
@@ -1894,7 +1950,7 @@
       </c>
       <c r="F20" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement NIST FIPS-validated cryptography for the following: to provision digital signatures, to generate cryptographic hashes, and to protect unclassified information requiring confidentiality and cryptographic protection in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
+          <t>Red Hat Enterprise Linux 9 must implement NIST FIPS-validated cryptography for the following: to provision digital signatures, to generate cryptographic hashes, and to protect unclassified information requiring confidentiality and cryptographic protection in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
         </is>
       </c>
       <c r="G20" s="2" t="inlineStr">
@@ -1943,7 +1999,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),SC-10,MA-4 e,AC-12</t>
+          <t>MA-4 e,AC-12,MA-4 (7),SC-10</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -1956,7 +2012,11 @@
           <t>SRG-OS-000126-GPOS-00066,SRG-OS-000163-GPOS-00072,SRG-OS-000279-GPOS-00109,SRG-OS-000395-GPOS-00175</t>
         </is>
       </c>
-      <c r="D21" s="2" t="inlineStr"/>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90811-1</t>
+        </is>
+      </c>
       <c r="E21" s="2" t="inlineStr">
         <is>
           <t>The operating system must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inactivity; and for user sessions (non-privileged session), the session must be terminated after 15 minutes of inactivity, except to fulfill documented and validated mission requirements.</t>
@@ -1964,7 +2024,7 @@
       </c>
       <c r="F21" s="2" t="inlineStr">
         <is>
-          <t>The operating system must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inacti</t>
+          <t>Red Hat Enterprise Linux 9 must terminate all network connections associated with a communications session at the end of the session, or as follows: for in-band management sessions (privileged sessions), the session must be terminated after 10 minutes of inacti</t>
         </is>
       </c>
       <c r="G21" s="2" t="inlineStr">
@@ -2014,7 +2074,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-14 (1),AU-12 a,AU-7 (1),CM-6 b,CM-5 (1),AU-6 (4),AU-3 (1),MA-4 (1) (a),AU-7 a</t>
+          <t>AU-3 (1),MA-4 (1) (a),CM-5 (1),CM-6 b,AU-7 (1),AU-14 (1),AU-12 a,AU-3,AU-7 a,AU-6 (4)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2027,7 +2087,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000038-GPOS-00016,SRG-OS-000039-GPOS-00017,SRG-OS-000040-GPOS-00018,SRG-OS-000041-GPOS-00019,SRG-OS-000042-GPOS-00021,SRG-OS-000051-GPOS-00024,SRG-OS-000054-GPOS-00025,SRG-OS-000122-GPOS-00063,SRG-OS-000254-GPOS-00095,SRG-OS-000255-GPOS-00096,SRG-OS-000365-GPOS-00152,SRG-OS-000392-GPOS-00172,SRG-OS-000480-GPOS-00227,SRG-OS-000062-GPOS-00031,SRG-OS-000349-GPOS-00137</t>
         </is>
       </c>
-      <c r="D22" s="2" t="inlineStr"/>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90829-3</t>
+        </is>
+      </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
           <t>The operating system must produce audit records containing information to establish the outcome of the events.</t>
@@ -2115,7 +2179,7 @@
       </c>
       <c r="F23" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow operating system admins to change security attributes on users, the operating system, or the operating systems components.</t>
+          <t>Red Hat Enterprise Linux 9 must allow operating system admins to change security attributes on users, the operating system, or the operating systems components.</t>
         </is>
       </c>
       <c r="G23" s="2" t="inlineStr">
@@ -2163,7 +2227,11 @@
           <t>SRG-OS-000278-GPOS-00108</t>
         </is>
       </c>
-      <c r="D24" s="2" t="inlineStr"/>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87757-1</t>
+        </is>
+      </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
           <t>The operating system must use cryptographic mechanisms to protect the integrity of audit tools.</t>
@@ -2171,7 +2239,7 @@
       </c>
       <c r="F24" s="2" t="inlineStr">
         <is>
-          <t>The operating system must use cryptographic mechanisms to protect the integrity of audit tools.</t>
+          <t>Red Hat Enterprise Linux 9 must use cryptographic mechanisms to protect the integrity of audit tools.</t>
         </is>
       </c>
       <c r="G24" s="2" t="inlineStr">
@@ -2243,7 +2311,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2256,7 +2324,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000064-GPOS-00033,SRG-OS-000458-GPOS-00203,SRG-OS-000461-GPOS-00205</t>
         </is>
       </c>
-      <c r="D25" s="2" t="inlineStr"/>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83786-4</t>
+        </is>
+      </c>
       <c r="E25" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to access categories of information (e.g., classification levels) occur.</t>
@@ -2264,7 +2336,7 @@
       </c>
       <c r="F25" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to access categories of information (e.g., classification levels) occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to access categories of information (e.g., classification levels) occur.</t>
         </is>
       </c>
       <c r="G25" s="2" t="inlineStr">
@@ -2325,7 +2397,11 @@
           <t>SRG-OS-000068-GPOS-00036</t>
         </is>
       </c>
-      <c r="D26" s="2" t="inlineStr"/>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89737-1</t>
+        </is>
+      </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
           <t>The operating system must map the authenticated identity to the user or group account for PKI-based authentication.</t>
@@ -2472,7 +2548,7 @@
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>The operating system must automatically terminate a user session after inactivity time-outs have expired or at shutdown.</t>
+          <t>Red Hat Enterprise Linux 9 must automatically terminate a user session after inactivity time-outs have expired or at shutdown.</t>
         </is>
       </c>
       <c r="G28" s="2" t="inlineStr">
@@ -2509,7 +2585,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8 (1),SC-8</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2522,7 +2598,11 @@
           <t>SRG-OS-000423-GPOS-00187,SRG-OS-000424-GPOS-00188,SRG-OS-000425-GPOS-00189,SRG-OS-000426-GPOS-00190</t>
         </is>
       </c>
-      <c r="D29" s="2" t="inlineStr"/>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90823-6</t>
+        </is>
+      </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect the confidentiality and integrity of transmitted information.</t>
@@ -2530,7 +2610,7 @@
       </c>
       <c r="F29" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect the confidentiality and integrity of transmitted information.</t>
+          <t>Red Hat Enterprise Linux 9 must protect the confidentiality and integrity of transmitted information.</t>
         </is>
       </c>
       <c r="G29" s="2" t="inlineStr">
@@ -2634,7 +2714,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -2647,7 +2727,11 @@
           <t>SRG-OS-000004-GPOS-00004,SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000304-GPOS-00121,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000470-GPOS-00214,SRG-OS-000471-GPOS-00215,SRG-OS-000239-GPOS-00089,SRG-OS-000240-GPOS-00090,SRG-OS-000241-GPOS-00091,SRG-OS-000303-GPOS-00120,SRG-OS-000304-GPOS-00121,SRG-OS-000466-GPOS-00210,SRG-OS-000476-GPOS-00221</t>
         </is>
       </c>
-      <c r="D31" s="2" t="inlineStr"/>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90176-9</t>
+        </is>
+      </c>
       <c r="E31" s="2" t="inlineStr">
         <is>
           <t>The operating system must audit all account removal actions.</t>
@@ -2655,7 +2739,7 @@
       </c>
       <c r="F31" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all account removal actions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all account removal actions.</t>
         </is>
       </c>
       <c r="G31" s="2" t="inlineStr">
@@ -2732,7 +2816,7 @@
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>The operating system must produce audit records containing information to establish what type of events occurred.</t>
+          <t>Red Hat Enterprise Linux 9 must produce audit records containing information to establish what type of events occurred.</t>
         </is>
       </c>
       <c r="G32" s="2" t="inlineStr">
@@ -2781,7 +2865,11 @@
           <t>SRG-OS-000480-GPOS-00226</t>
         </is>
       </c>
-      <c r="D33" s="2" t="inlineStr"/>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83635-3</t>
+        </is>
+      </c>
       <c r="E33" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce a delay of at least 4 seconds between logon prompts following a failed logon attempt.</t>
@@ -2789,7 +2877,7 @@
       </c>
       <c r="F33" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce a delay of at least 4 seconds between logon prompts following a failed logon attempt.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce a delay of at least 4 seconds between logon prompts following a failed logon attempt.</t>
         </is>
       </c>
       <c r="G33" s="2" t="inlineStr">
@@ -2838,7 +2926,7 @@
     <row r="34" ht="130" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -2851,7 +2939,11 @@
           <t>SRG-OS-000030-GPOS-00011,SRG-OS-000028-GPOS-00009</t>
         </is>
       </c>
-      <c r="D34" s="2" t="inlineStr"/>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83599-1</t>
+        </is>
+      </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide the capability for users to directly initiate a session lock for all connection types.</t>
@@ -2925,7 +3017,11 @@
           <t>SRG-OS-000077-GPOS-00045</t>
         </is>
       </c>
-      <c r="D35" s="2" t="inlineStr"/>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86354-8</t>
+        </is>
+      </c>
       <c r="E35" s="2" t="inlineStr">
         <is>
           <t>The operating system must prohibit password reuse for a minimum of five generations.</t>
@@ -2933,7 +3029,7 @@
       </c>
       <c r="F35" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prohibit password reuse for a minimum of five generations.</t>
+          <t>Red Hat Enterprise Linux 9 must prohibit password reuse for a minimum of five generations.</t>
         </is>
       </c>
       <c r="G35" s="2" t="inlineStr">
@@ -2996,7 +3092,11 @@
           <t>SRG-OS-000051-GPOS-00024</t>
         </is>
       </c>
-      <c r="D36" s="2" t="inlineStr"/>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83704-7</t>
+        </is>
+      </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
@@ -3004,7 +3104,7 @@
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
+          <t>Red Hat Enterprise Linux 9 must provide the capability to centrally review and analyze audit records from multiple components within the system.</t>
         </is>
       </c>
       <c r="G36" s="2" t="inlineStr">
@@ -3110,7 +3210,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>SI-11 b,AU-9</t>
+          <t>AU-9,SI-11 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3123,7 +3223,11 @@
           <t>SRG-OS-000057-GPOS-00027,SRG-OS-000058-GPOS-00028,SRG-OS-000059-GPOS-00029,SRG-OS-000206-GPOS-00084</t>
         </is>
       </c>
-      <c r="D38" s="2" t="inlineStr"/>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90516-6</t>
+        </is>
+      </c>
       <c r="E38" s="2" t="inlineStr">
         <is>
           <t>The operating system must reveal error messages only to authorized users.</t>
@@ -3131,7 +3235,7 @@
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>The operating system must reveal error messages only to authorized users.</t>
+          <t>Red Hat Enterprise Linux 9 must reveal error messages only to authorized users.</t>
         </is>
       </c>
       <c r="G38" s="2" t="inlineStr">
@@ -3191,7 +3295,11 @@
           <t>SRG-OS-000255-GPOS-00096,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D39" s="2" t="inlineStr"/>
+      <c r="D39" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83696-5</t>
+        </is>
+      </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
           <t>The operating system must produce audit records containing information to establish the identity of any individual or process associated with the event.</t>
@@ -3199,7 +3307,7 @@
       </c>
       <c r="F39" s="2" t="inlineStr">
         <is>
-          <t>The operating system must produce audit records containing information to establish the identity of any individual or process associated with the event.</t>
+          <t>Red Hat Enterprise Linux 9 must produce audit records containing information to establish the identity of any individual or process associated with the event.</t>
         </is>
       </c>
       <c r="G39" s="2" t="inlineStr">
@@ -3269,7 +3377,7 @@
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>The operating system must not alter original content or time ordering of audit records when it provides an audit reduction capability.</t>
+          <t>Red Hat Enterprise Linux 9 must not alter original content or time ordering of audit records when it provides an audit reduction capability.</t>
         </is>
       </c>
       <c r="G40" s="2" t="inlineStr">
@@ -3326,7 +3434,7 @@
       </c>
       <c r="F41" s="2" t="inlineStr">
         <is>
-          <t>The operating system must off-load audit records onto a different system or media from the system being audited.</t>
+          <t>Red Hat Enterprise Linux 9 must off-load audit records onto a different system or media from the system being audited.</t>
         </is>
       </c>
       <c r="G41" s="2" t="inlineStr">
@@ -3377,7 +3485,7 @@
     <row r="42" ht="130" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
@@ -3390,7 +3498,11 @@
           <t>SRG-OS-000405-GPOS-00184,SRG-OS-000185-GPOS-00079,SRG-OS-000404-GPOS-00183</t>
         </is>
       </c>
-      <c r="D42" s="2" t="inlineStr"/>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90849-1</t>
+        </is>
+      </c>
       <c r="E42" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement cryptographic mechanisms to prevent unauthorized modification of all information at rest on all operating system components.</t>
@@ -3398,7 +3510,7 @@
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to prevent unauthorized modification of all information at rest on all operating system components.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to prevent unauthorized modification of all information at rest on all operating system components.</t>
         </is>
       </c>
       <c r="G42" s="2" t="inlineStr">
@@ -3471,7 +3583,11 @@
           <t>SRG-OS-000027-GPOS-00008</t>
         </is>
       </c>
-      <c r="D43" s="2" t="inlineStr"/>
+      <c r="D43" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83641-1</t>
+        </is>
+      </c>
       <c r="E43" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit the number of concurrent sessions to ten for all accounts and/or account types.</t>
@@ -3479,7 +3595,7 @@
       </c>
       <c r="F43" s="2" t="inlineStr">
         <is>
-          <t>The operating system must limit the number of concurrent sessions to ten for all accounts and/or account types.</t>
+          <t>Red Hat Enterprise Linux 9 must limit the number of concurrent sessions to ten for all accounts and/or account types.</t>
         </is>
       </c>
       <c r="G43" s="2" t="inlineStr">
@@ -3542,7 +3658,11 @@
           <t>SRG-OS-000373-GPOS-00156,SRG-OS-000373-GPOS-00157,SRG-OS-000373-GPOS-00158</t>
         </is>
       </c>
-      <c r="D44" s="2" t="inlineStr"/>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83544-7</t>
+        </is>
+      </c>
       <c r="E44" s="2" t="inlineStr">
         <is>
           <t>The operating system must require users to re-authenticate when changing authenticators.</t>
@@ -3550,7 +3670,7 @@
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require users to re-authenticate when changing authenticators.</t>
+          <t>Red Hat Enterprise Linux 9 must require users to re-authenticate when changing authenticators.</t>
         </is>
       </c>
       <c r="G44" s="2" t="inlineStr">
@@ -3612,7 +3732,11 @@
           <t>SRG-OS-000023-GPOS-00006,SRG-OS-000024-GPOS-00007,SRG-OS-000228-GPOS-00088</t>
         </is>
       </c>
-      <c r="D45" s="2" t="inlineStr"/>
+      <c r="D45" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90807-9</t>
+        </is>
+      </c>
       <c r="E45" s="2" t="inlineStr">
         <is>
           <t>Any publically accessible connection to the operating system must display the Standard Mandatory DoD Notice and Consent Banner before granting access to the system.</t>
@@ -3620,7 +3744,7 @@
       </c>
       <c r="F45" s="2" t="inlineStr">
         <is>
-          <t>Any publically accessible connection to the operating system must display the Standard Mandatory DoD Notice and Consent Banner before granting access to the system.</t>
+          <t>Any publically accessible connection to Red Hat Enterprise Linux 9 must display the Standard Mandatory DoD Notice and Consent Banner before granting access to the system.</t>
         </is>
       </c>
       <c r="G45" s="2" t="inlineStr">
@@ -3718,7 +3842,7 @@
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to access security objects occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to access security objects occur.</t>
         </is>
       </c>
       <c r="G46" s="2" t="inlineStr">
@@ -3774,7 +3898,7 @@
       </c>
       <c r="F47" s="2" t="inlineStr">
         <is>
-          <t>The operating system must notify system administrators and ISSOs of account enabling actions.</t>
+          <t>Red Hat Enterprise Linux 9 must notify system administrators and ISSOs of account enabling actions.</t>
         </is>
       </c>
       <c r="G47" s="2" t="inlineStr">
@@ -3823,7 +3947,11 @@
           <t>SRG-OS-000480-GPOS-00228,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D48" s="2" t="inlineStr"/>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83644-5</t>
+        </is>
+      </c>
       <c r="E48" s="2" t="inlineStr">
         <is>
           <t>The operating system must define default permissions for all authenticated users in such a way that the user can only read and modify their own files.</t>
@@ -3831,7 +3959,7 @@
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>The operating system must define default permissions for all authenticated users in such a way that the user can only read and modify their own files.</t>
+          <t>Red Hat Enterprise Linux 9 must define default permissions for all authenticated users in such a way that the user can only read and modify their own files.</t>
         </is>
       </c>
       <c r="G48" s="2" t="inlineStr">
@@ -3903,7 +4031,7 @@
       </c>
       <c r="F49" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to prevent unauthorized disclosure of all information at rest on all operating system components.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to prevent unauthorized disclosure of all information at rest on all operating system components.</t>
         </is>
       </c>
       <c r="G49" s="2" t="inlineStr">
@@ -3938,7 +4066,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -3951,7 +4079,11 @@
           <t>SRG-OS-000109-GPOS-00056,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D50" s="2" t="inlineStr"/>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90800-4</t>
+        </is>
+      </c>
       <c r="E50" s="2" t="inlineStr">
         <is>
           <t>The operating system must require individuals to be authenticated with an individual authenticator prior to using a group authenticator.</t>
@@ -4033,7 +4165,7 @@
       </c>
       <c r="F51" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to prevent unauthorized disclosure of information and/or detect changes to information during transmission unless otherwise protected by alternative physical safeguards, such as, at a minimum, a</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to prevent unauthorized disclosure of information and/or detect changes to information during transmission unless otherwise protected by alternative physical safeguards, such as, at a minimum, a</t>
         </is>
       </c>
       <c r="G51" s="2" t="inlineStr">
@@ -4083,7 +4215,11 @@
           <t>SRG-OS-000120-GPOS-00061</t>
         </is>
       </c>
-      <c r="D52" s="2" t="inlineStr"/>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84221-1</t>
+        </is>
+      </c>
       <c r="E52" s="2" t="inlineStr">
         <is>
           <t>The operating system must use mechanisms meeting the requirements of applicable federal laws, Executive orders, directives, policies, regulations, standards, and guidance for authentication to a cryptographic module.</t>
@@ -4146,7 +4282,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4159,7 +4295,11 @@
           <t>SRG-OS-000396-GPOS-00176,SRG-OS-000393-GPOS-00173,SRG-OS-000394-GPOS-00174</t>
         </is>
       </c>
-      <c r="D53" s="2" t="inlineStr"/>
+      <c r="D53" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83450-7</t>
+        </is>
+      </c>
       <c r="E53" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement cryptographic mechanisms to protect the integrity of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
@@ -4167,7 +4307,7 @@
       </c>
       <c r="F53" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to protect the integrity of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to protect the integrity of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
         </is>
       </c>
       <c r="G53" s="2" t="inlineStr">
@@ -4296,7 +4436,11 @@
           <t>SRG-OS-000250-GPOS-00093,SRG-OS-000423-GPOS-00187</t>
         </is>
       </c>
-      <c r="D55" s="2" t="inlineStr"/>
+      <c r="D55" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86860-4</t>
+        </is>
+      </c>
       <c r="E55" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement cryptography to protect the integrity of remote access sessions.</t>
@@ -4304,7 +4448,7 @@
       </c>
       <c r="F55" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptography to protect the integrity of remote access sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptography to protect the integrity of remote access sessions.</t>
         </is>
       </c>
       <c r="G55" s="2" t="inlineStr">
@@ -4367,7 +4511,11 @@
           <t>SRG-OS-000392-GPOS-00172,SRG-OS-000470-GPOS-00214,SRG-OS-000473-GPOS-00218</t>
         </is>
       </c>
-      <c r="D56" s="2" t="inlineStr"/>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83783-1</t>
+        </is>
+      </c>
       <c r="E56" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful logon attempts occur.</t>
@@ -4375,7 +4523,7 @@
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful logon attempts occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful logon attempts occur.</t>
         </is>
       </c>
       <c r="G56" s="2" t="inlineStr">
@@ -4434,7 +4582,11 @@
           <t>SRG-OS-000433-GPOS-00192</t>
         </is>
       </c>
-      <c r="D57" s="2" t="inlineStr"/>
+      <c r="D57" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83970-4</t>
+        </is>
+      </c>
       <c r="E57" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement non-executable data to protect its memory from unauthorized code execution.</t>
@@ -4442,7 +4594,7 @@
       </c>
       <c r="F57" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement non-executable data to protect its memory from unauthorized code execution.</t>
+          <t>Red Hat Enterprise Linux 9 must implement non-executable data to protect its memory from unauthorized code execution.</t>
         </is>
       </c>
       <c r="G57" s="2" t="inlineStr">
@@ -4521,7 +4673,11 @@
           <t>SRG-OS-000029-GPOS-00010</t>
         </is>
       </c>
-      <c r="D58" s="2" t="inlineStr"/>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89876-7</t>
+        </is>
+      </c>
       <c r="E58" s="2" t="inlineStr">
         <is>
           <t>The operating system must initiate a session lock after a 15-minute period of inactivity for all connection types.</t>
@@ -4529,7 +4685,7 @@
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>The operating system must initiate a session lock after a 15-minute period of inactivity for all connection types.</t>
+          <t>Red Hat Enterprise Linux 9 must initiate a session lock after a 15-minute period of inactivity for all connection types.</t>
         </is>
       </c>
       <c r="G58" s="2" t="inlineStr">
@@ -4599,7 +4755,7 @@
       </c>
       <c r="F59" s="2" t="inlineStr">
         <is>
-          <t>The operating system must uniquely identify peripherals before establishing a connection.</t>
+          <t>Red Hat Enterprise Linux 9 must uniquely identify peripherals before establishing a connection.</t>
         </is>
       </c>
       <c r="G59" s="2" t="inlineStr">
@@ -4750,7 +4906,7 @@
       </c>
       <c r="F61" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide the capability for assigned IMOs/ISSOs or designated SAs to change the auditing to be performed on all operating system components, based on all selectable event criteria in near real time.</t>
+          <t>Red Hat Enterprise Linux 9 must provide the capability for assigned IMOs/ISSOs or designated SAs to change the auditing to be performed on all operating system components, based on all selectable event criteria in near real time.</t>
         </is>
       </c>
       <c r="G61" s="2" t="inlineStr">
@@ -4806,7 +4962,7 @@
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete privileges occur.</t>
         </is>
       </c>
       <c r="G62" s="2" t="inlineStr">
@@ -4841,7 +4997,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -4854,7 +5010,11 @@
           <t>SRG-OS-000046-GPOS-00022,SRG-OS-000343-GPOS-00134</t>
         </is>
       </c>
-      <c r="D63" s="2" t="inlineStr"/>
+      <c r="D63" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83698-1</t>
+        </is>
+      </c>
       <c r="E63" s="2" t="inlineStr">
         <is>
           <t>The operating system must immediately notify the SA and ISSO (at a minimum) when allocated audit record storage volume reaches 75% of the repository maximum audit record storage capacity.</t>
@@ -4862,7 +5022,7 @@
       </c>
       <c r="F63" s="2" t="inlineStr">
         <is>
-          <t>The operating system must immediately notify the SA and ISSO (at a minimum) when allocated audit record storage volume reaches 75% of the repository maximum audit record storage capacity.</t>
+          <t>Red Hat Enterprise Linux 9 must immediately notify the SA and ISSO (at a minimum) when allocated audit record storage volume reaches 75% of the repository maximum audit record storage capacity.</t>
         </is>
       </c>
       <c r="G63" s="2" t="inlineStr">
@@ -4942,7 +5102,7 @@
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>To prevent the compromise of authentication information, such as passwords during the authentication process, the feedback from the operating system must not provide any information allowing an unauthorized user to compromise the authentication mechanism.
+          <t>To prevent the compromise of authentication information, such as passwords during the authentication process, the feedback from Red Hat Enterprise Linux 9 must not provide any information allowing an unauthorized user to compromise the authentication mechanism.
 Obfuscation of user-provided information that is typed into the system is a method used when addressing this risk.
 For example, displaying asterisks when a user types in a password is an example of obscuring feedback of authentication information.</t>
         </is>
@@ -5005,7 +5165,11 @@
           <t>SRG-OS-000106-GPOS-00053,SRG-OS-000480-GPOS-00229,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D65" s="2" t="inlineStr"/>
+      <c r="D65" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90799-8</t>
+        </is>
+      </c>
       <c r="E65" s="2" t="inlineStr">
         <is>
           <t>The operating system must use multifactor authentication for network access to non-privileged accounts.</t>
@@ -5096,7 +5260,7 @@
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce password complexity by requiring that at least one special character be used.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce password complexity by requiring that at least one special character be used.</t>
         </is>
       </c>
       <c r="G66" s="2" t="inlineStr">
@@ -5132,7 +5296,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5145,7 +5309,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000458-GPOS-00203,SRG-OS-000462-GPOS-00206,SRG-OS-000463-GPOS-00207,SRG-OS-000471-GPOS-00215,SRG-OS-000474-GPOS-00219,SRG-OS-000466-GPOS-00210,SRG-OS-000064-GPOS-00033</t>
         </is>
       </c>
-      <c r="D67" s="2" t="inlineStr"/>
+      <c r="D67" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83821-9</t>
+        </is>
+      </c>
       <c r="E67" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to modify security objects occur.</t>
@@ -5153,7 +5321,7 @@
       </c>
       <c r="F67" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to modify security objects occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to modify security objects occur.</t>
         </is>
       </c>
       <c r="G67" s="2" t="inlineStr">
@@ -5224,7 +5392,7 @@
       </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>The operating system must limit the ability of non-privileged users to grant other users direct access to the contents of their home directories/folders.</t>
+          <t>Red Hat Enterprise Linux 9 must limit the ability of non-privileged users to grant other users direct access to the contents of their home directories/folders.</t>
         </is>
       </c>
       <c r="G68" s="2" t="inlineStr">
@@ -5258,7 +5426,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-7 b,AU-12 (3),AU-12 a,AU-12 c,AU-8 b,CM-6 b,CM-5 (1),AU-7 a</t>
+          <t>AU-12 (3),CM-5 (1),CM-6 b,AU-8 b,AU-12 c,AU-12 a,AU-7 a,AU-7 b</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5271,7 +5439,11 @@
           <t>SRG-OS-000122-GPOS-00063,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000359-GPOS-00146,SRG-OS-000365-GPOS-00152,SRG-OS-000474-GPOS-00219,SRG-OS-000475-GPOS-00220,SRG-OS-000480-GPOS-00227,SRG-OS-000062-GPOS-00031</t>
         </is>
       </c>
-      <c r="D69" s="2" t="inlineStr"/>
+      <c r="D69" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83649-4</t>
+        </is>
+      </c>
       <c r="E69" s="2" t="inlineStr">
         <is>
           <t>The operating system must produce audit records containing information to establish when (date and time) the events occurred.</t>
@@ -5342,7 +5514,11 @@
           <t>SRG-OS-000138-GPOS-00069</t>
         </is>
       </c>
-      <c r="D70" s="2" t="inlineStr"/>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83895-3</t>
+        </is>
+      </c>
       <c r="E70" s="2" t="inlineStr">
         <is>
           <t>Operating systems must prevent unauthorized and unintended information transfer via shared system resources.</t>
@@ -5421,7 +5597,11 @@
           <t>SRG-OS-000039-GPOS-00017,SRG-OS-000342-GPOS-00133,SRG-OS-000479-GPOS-00224</t>
         </is>
       </c>
-      <c r="D71" s="2" t="inlineStr"/>
+      <c r="D71" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83686-6</t>
+        </is>
+      </c>
       <c r="E71" s="2" t="inlineStr">
         <is>
           <t>The operating system must produce audit records containing information to establish where the events occurred.</t>
@@ -5571,7 +5751,7 @@
       </c>
       <c r="F73" s="2" t="inlineStr">
         <is>
-          <t>The operating system must not alter original content or time ordering of audit records when it provides a report generation capability.</t>
+          <t>Red Hat Enterprise Linux 9 must not alter original content or time ordering of audit records when it provides a report generation capability.</t>
         </is>
       </c>
       <c r="G73" s="2" t="inlineStr">
@@ -5620,7 +5800,11 @@
           <t>SRG-OS-000062-GPOS-00031</t>
         </is>
       </c>
-      <c r="D74" s="2" t="inlineStr"/>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84206-2</t>
+        </is>
+      </c>
       <c r="E74" s="2" t="inlineStr">
         <is>
           <t>The operating system must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
@@ -5628,7 +5812,7 @@
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
+          <t>Red Hat Enterprise Linux 9 must provide audit record generation capability for DoD-defined auditable events for all operating system components.</t>
         </is>
       </c>
       <c r="G74" s="2" t="inlineStr">
@@ -5765,7 +5949,7 @@
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement NSA-approved cryptography to protect classified information in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
+          <t>Red Hat Enterprise Linux 9 must implement NSA-approved cryptography to protect classified information in accordance with applicable federal laws, Executive Orders, directives, policies, regulations, and standards.</t>
         </is>
       </c>
       <c r="G76" s="2" t="inlineStr">
@@ -5799,7 +5983,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AC-2 (4),AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -5812,7 +5996,11 @@
           <t>SRG-OS-000004-GPOS-00004,SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000304-GPOS-00121,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000470-GPOS-00214,SRG-OS-000471-GPOS-00215,SRG-OS-000239-GPOS-00089,SRG-OS-000240-GPOS-00090,SRG-OS-000241-GPOS-00091,SRG-OS-000303-GPOS-00120,SRG-OS-000304-GPOS-00121,SRG-OS-000466-GPOS-00210,SRG-OS-000476-GPOS-00221,SRG-OS-000274-GPOS-00104,SRG-OS-000275-GPOS-00105,SRG-OS-000276-GPOS-00106,SRG-OS-000277-GPOS-00107</t>
         </is>
       </c>
-      <c r="D77" s="2" t="inlineStr"/>
+      <c r="D77" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83714-6</t>
+        </is>
+      </c>
       <c r="E77" s="2" t="inlineStr">
         <is>
           <t>The operating system must notify system administrators and ISSOs when accounts are removed.</t>
@@ -5899,7 +6087,11 @@
           <t>SRG-OS-000125-GPOS-00065</t>
         </is>
       </c>
-      <c r="D78" s="2" t="inlineStr"/>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86722-6</t>
+        </is>
+      </c>
       <c r="E78" s="2" t="inlineStr">
         <is>
           <t>The operating system must employ strong authenticators in the establishment of nonlocal maintenance and diagnostic sessions.</t>
@@ -5964,7 +6156,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -5977,7 +6169,11 @@
           <t>SRG-OS-000256-GPOS-00097,SRG-OS-000257-GPOS-00098,SRG-OS-000258-GPOS-00099,SRG-OS-000278-GPOS-00108</t>
         </is>
       </c>
-      <c r="D79" s="2" t="inlineStr"/>
+      <c r="D79" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90840-0</t>
+        </is>
+      </c>
       <c r="E79" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect audit tools from unauthorized deletion.</t>
@@ -5985,7 +6181,7 @@
       </c>
       <c r="F79" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit tools from unauthorized deletion.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit tools from unauthorized deletion.</t>
         </is>
       </c>
       <c r="G79" s="2" t="inlineStr">
@@ -6035,7 +6231,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (4),IA-2 (2),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2 (1),IA-2 (4),IA-2 (3)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6135,7 +6331,11 @@
           <t>SRG-OS-000480-GPOS-00227,SRG-OS-000366-GPOS-00153</t>
         </is>
       </c>
-      <c r="D81" s="2" t="inlineStr"/>
+      <c r="D81" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83954-8</t>
+        </is>
+      </c>
       <c r="E81" s="2" t="inlineStr">
         <is>
           <t>The operating system must prevent the installation of patches, service packs, device drivers, or operating system components without verification they have been digitally signed using a certificate that is recognized and approved by the organization.</t>
@@ -6143,7 +6343,7 @@
       </c>
       <c r="F81" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent the installation of patches, service packs, device drivers, or operating system components without verification they have been digitally signed using a certificate that is recognized and approved by the organization.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent the installation of patches, service packs, device drivers, or operating system components without verification they have been digitally signed using a certificate that is recognized and approved by the organization.</t>
         </is>
       </c>
       <c r="G81" s="2" t="inlineStr">
@@ -6228,7 +6428,7 @@
       </c>
       <c r="F82" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to access privileges occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to access privileges occur.</t>
         </is>
       </c>
       <c r="G82" s="2" t="inlineStr">
@@ -6341,7 +6541,7 @@
       </c>
       <c r="F84" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect against or limit the effects of Denial of Service (DoS) attacks by ensuring the operating system is implementing rate-limiting measures on impacted network interfaces.</t>
+          <t>Red Hat Enterprise Linux 9 must protect against or limit the effects of Denial of Service (DoS) attacks by ensuring the operating system is implementing rate-limiting measures on impacted network interfaces.</t>
         </is>
       </c>
       <c r="G84" s="2" t="inlineStr">
@@ -6420,7 +6620,7 @@
       </c>
       <c r="F85" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent all software from executing at higher privilege levels than users executing the software.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent all software from executing at higher privilege levels than users executing the software.</t>
         </is>
       </c>
       <c r="G85" s="2" t="inlineStr">
@@ -6455,7 +6655,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6468,7 +6668,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000064-GPOS-00033,SRG-OS-000466-GPOS-00210,SRG-OS-000458-GPOS-00203,SRG-OS-000474-GPOS-00219</t>
         </is>
       </c>
-      <c r="D86" s="2" t="inlineStr"/>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83812-8</t>
+        </is>
+      </c>
       <c r="E86" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful accesses to objects occur.</t>
@@ -6476,7 +6680,7 @@
       </c>
       <c r="F86" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful accesses to objects occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful accesses to objects occur.</t>
         </is>
       </c>
       <c r="G86" s="2" t="inlineStr">
@@ -6539,7 +6743,11 @@
           <t>SRG-OS-000073-GPOS-00041</t>
         </is>
       </c>
-      <c r="D87" s="2" t="inlineStr"/>
+      <c r="D87" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88865-1</t>
+        </is>
+      </c>
       <c r="E87" s="2" t="inlineStr">
         <is>
           <t>The operating system must store only encrypted representations of passwords.</t>
@@ -6547,7 +6755,7 @@
       </c>
       <c r="F87" s="2" t="inlineStr">
         <is>
-          <t>The operating system must store only encrypted representations of passwords.</t>
+          <t>Red Hat Enterprise Linux 9 must store only encrypted representations of passwords.</t>
         </is>
       </c>
       <c r="G87" s="2" t="inlineStr">
@@ -6601,7 +6809,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AC-2 (4),AC-6 (9),AU-12 c</t>
+          <t>CM-5 (1),AU-12 c,AC-6 (9),AC-2 (4)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6622,7 +6830,7 @@
       </c>
       <c r="F88" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records showing starting and ending time for user access to the system.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records showing starting and ending time for user access to the system.</t>
         </is>
       </c>
       <c r="G88" s="2" t="inlineStr">
@@ -6668,7 +6876,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (5),IA-2 (2),IA-2 (3),IA-2</t>
+          <t>IA-2,IA-2 (4),IA-2 (2),IA-2 (3),IA-2 (5)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6681,7 +6889,11 @@
           <t>SRG-OS-000104-GPOS-00051,SRG-OS-000106-GPOS-00053,SRG-OS-000107-GPOS-00054,SRG-OS-000109-GPOS-00056,SRG-OS-000108-GPOS-00055,SRG-OS-000108-GPOS-00057,SRG-OS-000108-GPOS-00058</t>
         </is>
       </c>
-      <c r="D89" s="2" t="inlineStr"/>
+      <c r="D89" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89122-6</t>
+        </is>
+      </c>
       <c r="E89" s="2" t="inlineStr">
         <is>
           <t>The operating system must uniquely identify and must authenticate organizational users (or processes acting on behalf of organizational users).</t>
@@ -6748,7 +6960,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (11),IA-2 (12)</t>
+          <t>IA-2 (12),IA-2 (11)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -6761,7 +6973,11 @@
           <t>SRG-OS-000375-GPOS-00160,SRG-OS-000377-GPOS-00162</t>
         </is>
       </c>
-      <c r="D90" s="2" t="inlineStr"/>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87088-1</t>
+        </is>
+      </c>
       <c r="E90" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
@@ -6769,7 +6985,7 @@
       </c>
       <c r="F90" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
+          <t>Red Hat Enterprise Linux 9 must implement multifactor authentication for remote access to privileged accounts in such a way that one of the factors is provided by a device separate from the system gaining access.</t>
         </is>
       </c>
       <c r="G90" s="2" t="inlineStr">
@@ -6824,7 +7040,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9 (3),AU-9</t>
+          <t>AU-9,AU-9 (3)</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -6837,7 +7053,11 @@
           <t>SRG-OS-000256-GPOS-00097,SRG-OS-000257-GPOS-00098,SRG-OS-000278-GPOS-00108</t>
         </is>
       </c>
-      <c r="D91" s="2" t="inlineStr"/>
+      <c r="D91" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90842-6</t>
+        </is>
+      </c>
       <c r="E91" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect audit tools from unauthorized modification.</t>
@@ -6845,7 +7065,7 @@
       </c>
       <c r="F91" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit tools from unauthorized modification.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit tools from unauthorized modification.</t>
         </is>
       </c>
       <c r="G91" s="2" t="inlineStr">
@@ -7008,7 +7228,7 @@
       </c>
       <c r="F93" s="2" t="inlineStr">
         <is>
-          <t>The operating system must, at a minimum, off-load audit data from interconnected systems in real time and off-load audit data from standalone systems weekly.</t>
+          <t>Red Hat Enterprise Linux 9 must, at a minimum, off-load audit data from interconnected systems in real time and off-load audit data from standalone systems weekly.</t>
         </is>
       </c>
       <c r="G93" s="2" t="inlineStr">
@@ -7056,7 +7276,11 @@
           <t>SRG-OS-000075-GPOS-00043</t>
         </is>
       </c>
-      <c r="D94" s="2" t="inlineStr"/>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83610-6</t>
+        </is>
+      </c>
       <c r="E94" s="2" t="inlineStr">
         <is>
           <t>Operating systems must enforce 24 hours/1 day as the minimum password lifetime.</t>
@@ -7133,7 +7357,11 @@
           <t>SRG-OS-000072-GPOS-00040</t>
         </is>
       </c>
-      <c r="D95" s="2" t="inlineStr"/>
+      <c r="D95" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83564-5</t>
+        </is>
+      </c>
       <c r="E95" s="2" t="inlineStr">
         <is>
           <t>The operating system must require the change of at least 50% of the total number of characters when passwords are changed.</t>
@@ -7141,7 +7369,7 @@
       </c>
       <c r="F95" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require the change of at least 50% of the total number of characters when passwords are changed.</t>
+          <t>Red Hat Enterprise Linux 9 must require the change of at least 50% of the total number of characters when passwords are changed.</t>
         </is>
       </c>
       <c r="G95" s="2" t="inlineStr">
@@ -7198,7 +7426,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8 (1),SC-8</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7211,7 +7439,11 @@
           <t>SRG-OS-000299-GPOS-00117,SRG-OS-000300-GPOS-00118,SRG-OS-000424-GPOS-00188,SRG-OS-000481-GPOS-000481</t>
         </is>
       </c>
-      <c r="D96" s="2" t="inlineStr"/>
+      <c r="D96" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84066-0</t>
+        </is>
+      </c>
       <c r="E96" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect wireless access to and from the system using encryption.</t>
@@ -7219,7 +7451,7 @@
       </c>
       <c r="F96" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect wireless access to and from the system using encryption.</t>
+          <t>Red Hat Enterprise Linux 9 must protect wireless access to and from the system using encryption.</t>
         </is>
       </c>
       <c r="G96" s="2" t="inlineStr">
@@ -7274,7 +7506,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-8 (1) (a),AU-8 (1) (b)</t>
+          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7287,7 +7519,11 @@
           <t>SRG-OS-000355-GPOS-00143,SRG-OS-000356-GPOS-00144,SRG-OS-000359-GPOS-00146</t>
         </is>
       </c>
-      <c r="D97" s="2" t="inlineStr"/>
+      <c r="D97" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88648-1</t>
+        </is>
+      </c>
       <c r="E97" s="2" t="inlineStr">
         <is>
           <t>The operating system must synchronize internal information system clocks to the authoritative time source when the time difference is greater than one second.</t>
@@ -7295,7 +7531,7 @@
       </c>
       <c r="F97" s="2" t="inlineStr">
         <is>
-          <t>The operating system must synchronize internal information system clocks to the authoritative time source when the time difference is greater than one second.</t>
+          <t>Red Hat Enterprise Linux 9 must synchronize internal information system clocks to the authoritative time source when the time difference is greater than one second.</t>
         </is>
       </c>
       <c r="G97" s="2" t="inlineStr">
@@ -7360,7 +7596,11 @@
           <t>SRG-OS-000259-GPOS-00100</t>
         </is>
       </c>
-      <c r="D98" s="2" t="inlineStr"/>
+      <c r="D98" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89858-5</t>
+        </is>
+      </c>
       <c r="E98" s="2" t="inlineStr">
         <is>
           <t>The operating system must limit privileges to change software resident within software libraries.</t>
@@ -7368,7 +7608,7 @@
       </c>
       <c r="F98" s="2" t="inlineStr">
         <is>
-          <t>The operating system must limit privileges to change software resident within software libraries.</t>
+          <t>Red Hat Enterprise Linux 9 must limit privileges to change software resident within software libraries.</t>
         </is>
       </c>
       <c r="G98" s="2" t="inlineStr">
@@ -7435,7 +7675,11 @@
           <t>SRG-OS-000057-GPOS-00027,SRG-OS-000058-GPOS-00028,SRG-OS-000059-GPOS-00029</t>
         </is>
       </c>
-      <c r="D99" s="2" t="inlineStr"/>
+      <c r="D99" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83716-1</t>
+        </is>
+      </c>
       <c r="E99" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect audit information from unauthorized read access.</t>
@@ -7443,7 +7687,7 @@
       </c>
       <c r="F99" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit information from unauthorized read access.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit information from unauthorized read access.</t>
         </is>
       </c>
       <c r="G99" s="2" t="inlineStr">
@@ -7584,7 +7828,11 @@
           <t>SRG-OS-000373-GPOS-00156,SRG-OS-000312-GPOS-00123</t>
         </is>
       </c>
-      <c r="D101" s="2" t="inlineStr"/>
+      <c r="D101" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90085-2</t>
+        </is>
+      </c>
       <c r="E101" s="2" t="inlineStr">
         <is>
           <t>The operating system must require users to re-authenticate for privilege escalation.</t>
@@ -7592,7 +7840,7 @@
       </c>
       <c r="F101" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require users to re-authenticate for privilege escalation.</t>
+          <t>Red Hat Enterprise Linux 9 must require users to re-authenticate for privilege escalation.</t>
         </is>
       </c>
       <c r="G101" s="2" t="inlineStr">
@@ -7641,7 +7889,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -7654,7 +7902,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000471-GPOS-00216,SRG-OS-000477-GPOS-00222</t>
         </is>
       </c>
-      <c r="D102" s="2" t="inlineStr"/>
+      <c r="D102" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83802-9</t>
+        </is>
+      </c>
       <c r="E102" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records for all kernel module load, unload, and restart actions, and also for all program initiations.</t>
@@ -7662,7 +7914,7 @@
       </c>
       <c r="F102" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records for all kernel module load, unload, and restart actions, and also for all program initiations.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records for all kernel module load, unload, and restart actions, and also for all program initiations.</t>
         </is>
       </c>
       <c r="G102" s="2" t="inlineStr">
@@ -7809,7 +8061,7 @@
       </c>
       <c r="F104" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all account enabling actions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all account enabling actions.</t>
         </is>
       </c>
       <c r="G104" s="2" t="inlineStr">
@@ -7857,7 +8109,11 @@
           <t>SRG-OS-000327-GPOS-00127</t>
         </is>
       </c>
-      <c r="D105" s="2" t="inlineStr"/>
+      <c r="D105" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83759-1</t>
+        </is>
+      </c>
       <c r="E105" s="2" t="inlineStr">
         <is>
           <t>The operating system must audit the execution of privileged functions.</t>
@@ -7865,7 +8121,7 @@
       </c>
       <c r="F105" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit the execution of privileged functions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit the execution of privileged functions.</t>
         </is>
       </c>
       <c r="G105" s="2" t="inlineStr">
@@ -7945,7 +8201,7 @@
       </c>
       <c r="F106" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records for all direct access to the information system.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records for all direct access to the information system.</t>
         </is>
       </c>
       <c r="G106" s="2" t="inlineStr">
@@ -8001,7 +8257,7 @@
       </c>
       <c r="F107" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide a report generation capability that supports on-demand reporting requirements.</t>
+          <t>Red Hat Enterprise Linux 9 must provide a report generation capability that supports on-demand reporting requirements.</t>
         </is>
       </c>
       <c r="G107" s="2" t="inlineStr">
@@ -8057,7 +8313,7 @@
       </c>
       <c r="F108" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit information from unauthorized deletion.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit information from unauthorized deletion.</t>
         </is>
       </c>
       <c r="G108" s="2" t="inlineStr">
@@ -8191,7 +8447,7 @@
       </c>
       <c r="F110" s="2" t="inlineStr">
         <is>
-          <t>The operating system must maintain the confidentiality and integrity of information during reception.</t>
+          <t>Red Hat Enterprise Linux 9 must maintain the confidentiality and integrity of information during reception.</t>
         </is>
       </c>
       <c r="G110" s="2" t="inlineStr">
@@ -8240,7 +8496,11 @@
           <t>SRG-OS-000046-GPOS-00022,SRG-OS-000047-GPOS-00023</t>
         </is>
       </c>
-      <c r="D111" s="2" t="inlineStr"/>
+      <c r="D111" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83709-6</t>
+        </is>
+      </c>
       <c r="E111" s="2" t="inlineStr">
         <is>
           <t>The operating system must shut down by default upon audit failure (unless availability is an overriding concern).</t>
@@ -8248,7 +8508,7 @@
       </c>
       <c r="F111" s="2" t="inlineStr">
         <is>
-          <t>The operating system must shut down by default upon audit failure (unless availability is an overriding concern).</t>
+          <t>Red Hat Enterprise Linux 9 must shut down by default upon audit failure (unless availability is an overriding concern).</t>
         </is>
       </c>
       <c r="G111" s="2" t="inlineStr">
@@ -8325,7 +8585,7 @@
       </c>
       <c r="F112" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when concurrent logons to the same account occur from different sources.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when concurrent logons to the same account occur from different sources.</t>
         </is>
       </c>
       <c r="G112" s="2" t="inlineStr">
@@ -8381,7 +8641,7 @@
       </c>
       <c r="F113" s="2" t="inlineStr">
         <is>
-          <t>The operating system must allow operating system admins to grant their privileges to other operating system admins.</t>
+          <t>Red Hat Enterprise Linux 9 must allow operating system admins to grant their privileges to other operating system admins.</t>
         </is>
       </c>
       <c r="G113" s="2" t="inlineStr">
@@ -8437,7 +8697,7 @@
       </c>
       <c r="F114" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide a report generation capability that supports after-the-fact investigations of security incidents.</t>
+          <t>Red Hat Enterprise Linux 9 must provide a report generation capability that supports after-the-fact investigations of security incidents.</t>
         </is>
       </c>
       <c r="G114" s="2" t="inlineStr">
@@ -8576,7 +8836,7 @@
       </c>
       <c r="F116" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">The operating system must notify system administrators and ISSOs when accounts are disabled. </t>
+          <t xml:space="preserve">Red Hat Enterprise Linux 9 must notify system administrators and ISSOs when accounts are disabled. </t>
         </is>
       </c>
       <c r="G116" s="2" t="inlineStr">
@@ -8629,7 +8889,11 @@
           <t>SRG-OS-000437-GPOS-00194</t>
         </is>
       </c>
-      <c r="D117" s="2" t="inlineStr"/>
+      <c r="D117" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83458-0</t>
+        </is>
+      </c>
       <c r="E117" s="2" t="inlineStr">
         <is>
           <t>The operating system must remove all software components after updated versions have been installed.</t>
@@ -8769,7 +9033,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -8782,7 +9046,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000458-GPOS-00203,SRG-OS-000462-GPOS-00206,SRG-OS-000463-GPOS-00207,SRG-OS-000468-GPOS-00212,SRG-OS-000471-GPOS-00215,SRG-OS-000474-GPOS-00219,SRG-OS-000064-GPOS-00033</t>
         </is>
       </c>
-      <c r="D119" s="2" t="inlineStr"/>
+      <c r="D119" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83817-7</t>
+        </is>
+      </c>
       <c r="E119" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to delete security objects occur.</t>
@@ -8790,7 +9058,7 @@
       </c>
       <c r="F119" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to delete security objects occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete security objects occur.</t>
         </is>
       </c>
       <c r="G119" s="2" t="inlineStr">
@@ -8936,7 +9204,7 @@
       </c>
       <c r="F121" s="2" t="inlineStr">
         <is>
-          <t>The operating system must behave in a predictable and documented manner that reflects organizational and system objectives when invalid inputs are received.</t>
+          <t>Red Hat Enterprise Linux 9 must behave in a predictable and documented manner that reflects organizational and system objectives when invalid inputs are received.</t>
         </is>
       </c>
       <c r="G121" s="2" t="inlineStr">
@@ -9005,7 +9273,11 @@
           <t>SRG-OS-000378-GPOS-00163</t>
         </is>
       </c>
-      <c r="D122" s="2" t="inlineStr"/>
+      <c r="D122" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84203-9</t>
+        </is>
+      </c>
       <c r="E122" s="2" t="inlineStr">
         <is>
           <t>The operating system must authenticate peripherals before establishing a connection.</t>
@@ -9013,7 +9285,7 @@
       </c>
       <c r="F122" s="2" t="inlineStr">
         <is>
-          <t>The operating system must authenticate peripherals before establishing a connection.</t>
+          <t>Red Hat Enterprise Linux 9 must authenticate peripherals before establishing a connection.</t>
         </is>
       </c>
       <c r="G122" s="2" t="inlineStr">
@@ -9072,7 +9344,11 @@
           <t>SRG-OS-000096-GPOS-00050,SRG-OS-000095-GPOS-00049</t>
         </is>
       </c>
-      <c r="D123" s="2" t="inlineStr"/>
+      <c r="D123" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87543-5</t>
+        </is>
+      </c>
       <c r="E123" s="2" t="inlineStr">
         <is>
           <t>The operating system must be configured to prohibit or restrict the use of functions, ports, protocols, and/or services, as defined in the PPSM CAL and vulnerability assessments.</t>
@@ -9080,7 +9356,7 @@
       </c>
       <c r="F123" s="2" t="inlineStr">
         <is>
-          <t>The operating system must be configured to prohibit or restrict the use of functions, ports, protocols, and/or services, as defined in the PPSM CAL and vulnerability assessments.</t>
+          <t>Red Hat Enterprise Linux 9 must be configured to prohibit or restrict the use of functions, ports, protocols, and/or services, as defined in the PPSM CAL and vulnerability assessments.</t>
         </is>
       </c>
       <c r="G123" s="2" t="inlineStr">
@@ -9129,7 +9405,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9142,7 +9418,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000466-GPOS-00210,SRG-OS-000467-GPOS-00211,SRG-OS-000468-GPOS-00212</t>
         </is>
       </c>
-      <c r="D124" s="2" t="inlineStr"/>
+      <c r="D124" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83754-2</t>
+        </is>
+      </c>
       <c r="E124" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to delete security levels occur.</t>
@@ -9150,7 +9430,7 @@
       </c>
       <c r="F124" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to delete security levels occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to delete security levels occur.</t>
         </is>
       </c>
       <c r="G124" s="2" t="inlineStr">
@@ -9212,7 +9492,11 @@
           <t>SRG-OS-000095-GPOS-00049,SRG-OS-000300-GPOS-00118</t>
         </is>
       </c>
-      <c r="D125" s="2" t="inlineStr"/>
+      <c r="D125" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84067-8</t>
+        </is>
+      </c>
       <c r="E125" s="2" t="inlineStr">
         <is>
           <t>The operating system must protect wireless access to the system using authentication of users and/or devices.</t>
@@ -9220,7 +9504,7 @@
       </c>
       <c r="F125" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect wireless access to the system using authentication of users and/or devices.</t>
+          <t>Red Hat Enterprise Linux 9 must protect wireless access to the system using authentication of users and/or devices.</t>
         </is>
       </c>
       <c r="G125" s="2" t="inlineStr">
@@ -9293,7 +9577,7 @@
       </c>
       <c r="F126" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all account disabling actions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all account disabling actions.</t>
         </is>
       </c>
       <c r="G126" s="2" t="inlineStr">
@@ -9349,7 +9633,7 @@
       </c>
       <c r="F127" s="2" t="inlineStr">
         <is>
-          <t>The operating system must record time stamps for audit records that meet a minimum granularity of one second for a minimum degree of precision.</t>
+          <t>Red Hat Enterprise Linux 9 must record time stamps for audit records that meet a minimum granularity of one second for a minimum degree of precision.</t>
         </is>
       </c>
       <c r="G127" s="2" t="inlineStr">
@@ -9384,7 +9668,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (c),CM-7 a</t>
+          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -9397,7 +9681,11 @@
           <t>SRG-OS-000074-GPOS-00042,SRG-OS-000095-GPOS-00049,SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D128" s="2" t="inlineStr"/>
+      <c r="D128" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84159-3</t>
+        </is>
+      </c>
       <c r="E128" s="2" t="inlineStr">
         <is>
           <t>The operating system must transmit only encrypted representations of passwords.</t>
@@ -9611,7 +9899,11 @@
           <t>SRG-OS-000071-GPOS-00039</t>
         </is>
       </c>
-      <c r="D131" s="2" t="inlineStr"/>
+      <c r="D131" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83566-0</t>
+        </is>
+      </c>
       <c r="E131" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce password complexity by requiring that at least one numeric character be used.</t>
@@ -9701,7 +9993,7 @@
       </c>
       <c r="F132" s="2" t="inlineStr">
         <is>
-          <t>The operating system must authenticate all endpoint devices before establishing a local, remote, and/or network connection using bidirectional authentication that is cryptographically based.</t>
+          <t>Red Hat Enterprise Linux 9 must authenticate all endpoint devices before establishing a local, remote, and/or network connection using bidirectional authentication that is cryptographically based.</t>
         </is>
       </c>
       <c r="G132" s="2" t="inlineStr">
@@ -9816,7 +10108,11 @@
           <t>SRG-OS-000046-GPOS-00022</t>
         </is>
       </c>
-      <c r="D134" s="2" t="inlineStr"/>
+      <c r="D134" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90826-9</t>
+        </is>
+      </c>
       <c r="E134" s="2" t="inlineStr">
         <is>
           <t>The operating system must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
@@ -9824,7 +10120,7 @@
       </c>
       <c r="F134" s="2" t="inlineStr">
         <is>
-          <t>The operating system must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
+          <t>Red Hat Enterprise Linux 9 must alert the ISSO and SA (at a minimum) in the event of an audit processing failure.</t>
         </is>
       </c>
       <c r="G134" s="2" t="inlineStr">
@@ -9888,7 +10184,11 @@
           <t>SRG-OS-000080-GPOS-00048</t>
         </is>
       </c>
-      <c r="D135" s="2" t="inlineStr"/>
+      <c r="D135" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83592-6</t>
+        </is>
+      </c>
       <c r="E135" s="2" t="inlineStr">
         <is>
           <t>The operating system must enforce approved authorizations for logical access to information and system resources in accordance with applicable access control policies.</t>
@@ -9896,7 +10196,7 @@
       </c>
       <c r="F135" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce approved authorizations for logical access to information and system resources in accordance with applicable access control policies.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce approved authorizations for logical access to information and system resources in accordance with applicable access control policies.</t>
         </is>
       </c>
       <c r="G135" s="2" t="inlineStr">
@@ -9946,7 +10246,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -9959,7 +10259,11 @@
           <t>SRG-OS-000031-GPOS-00012,SRG-OS-000028-GPOS-00009</t>
         </is>
       </c>
-      <c r="D136" s="2" t="inlineStr"/>
+      <c r="D136" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90586-9</t>
+        </is>
+      </c>
       <c r="E136" s="2" t="inlineStr">
         <is>
           <t>The operating system must retain a users session lock until that user reestablishes access using established identification and authentication procedures.</t>
@@ -10054,7 +10358,7 @@
       </c>
       <c r="F137" s="2" t="inlineStr">
         <is>
-          <t>The operating system must notify system administrators and ISSOs when accounts are created.</t>
+          <t>Red Hat Enterprise Linux 9 must notify system administrators and ISSOs when accounts are created.</t>
         </is>
       </c>
       <c r="G137" s="2" t="inlineStr">
@@ -10180,7 +10484,11 @@
           <t>SRG-OS-000363-GPOS-00150,SRG-OS-000446-GPOS-00200,SRG-OS-000447-GPOS-00201</t>
         </is>
       </c>
-      <c r="D139" s="2" t="inlineStr"/>
+      <c r="D139" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83437-4</t>
+        </is>
+      </c>
       <c r="E139" s="2" t="inlineStr">
         <is>
           <t>The operating system must perform verification of the correct operation of security functions: upon system start-up and/or restart; upon command by a user with privileged access; and/or every 30 days.</t>
@@ -10188,7 +10496,7 @@
       </c>
       <c r="F139" s="2" t="inlineStr">
         <is>
-          <t>The operating system must perform verification of the correct operation of security functions: upon system start-up and/or restart; upon command by a user with privileged access; and/or every 30 days.</t>
+          <t>Red Hat Enterprise Linux 9 must perform verification of the correct operation of security functions: upon system start-up and/or restart; upon command by a user with privileged access; and/or every 30 days.</t>
         </is>
       </c>
       <c r="G139" s="2" t="inlineStr">
@@ -10268,7 +10576,7 @@
       </c>
       <c r="F140" s="2" t="inlineStr">
         <is>
-          <t>The operating system must be configured to disable non-essential capabilities.</t>
+          <t>Red Hat Enterprise Linux 9 must be configured to disable non-essential capabilities.</t>
         </is>
       </c>
       <c r="G140" s="2" t="inlineStr">
@@ -10325,7 +10633,7 @@
       </c>
       <c r="F141" s="2" t="inlineStr">
         <is>
-          <t>The operating system must provide an audit reduction capability that supports on-demand audit review and analysis.</t>
+          <t>Red Hat Enterprise Linux 9 must provide an audit reduction capability that supports on-demand audit review and analysis.</t>
         </is>
       </c>
       <c r="G141" s="2" t="inlineStr">
@@ -10373,7 +10681,11 @@
           <t>SRG-OS-000123-GPOS-00064,SRG-OS-000002-GPOS-00002</t>
         </is>
       </c>
-      <c r="D142" s="2" t="inlineStr"/>
+      <c r="D142" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90560-4</t>
+        </is>
+      </c>
       <c r="E142" s="2" t="inlineStr">
         <is>
           <t>The operating system must automatically remove or disable temporary user accounts after 72 hours.</t>
@@ -10692,7 +11004,7 @@
       </c>
       <c r="F146" s="2" t="inlineStr">
         <is>
-          <t>The operating system must control remote access methods.</t>
+          <t>Red Hat Enterprise Linux 9 must control remote access methods.</t>
         </is>
       </c>
       <c r="G146" s="2" t="inlineStr">
@@ -10741,7 +11053,11 @@
           <t>SRG-OS-000032-GPOS-00013</t>
         </is>
       </c>
-      <c r="D147" s="2" t="inlineStr"/>
+      <c r="D147" s="2" t="inlineStr">
+        <is>
+          <t>CCE-86923-0</t>
+        </is>
+      </c>
       <c r="E147" s="2" t="inlineStr">
         <is>
           <t>The operating system must monitor remote access methods.</t>
@@ -10809,7 +11125,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-14 (1),AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -10822,7 +11138,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000471-GPOS-00215,SRG-OS-000473-GPOS-00218,SRG-OS-000254-GPOS-00095</t>
         </is>
       </c>
-      <c r="D148" s="2" t="inlineStr"/>
+      <c r="D148" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83651-0</t>
+        </is>
+      </c>
       <c r="E148" s="2" t="inlineStr">
         <is>
           <t>The operating system must initiate session audits at system start-up.</t>
@@ -10830,7 +11150,7 @@
       </c>
       <c r="F148" s="2" t="inlineStr">
         <is>
-          <t>The operating system must initiate session audits at system start-up.</t>
+          <t>Red Hat Enterprise Linux 9 must initiate session audits at system start-up.</t>
         </is>
       </c>
       <c r="G148" s="2" t="inlineStr">
@@ -10957,7 +11277,11 @@
           <t>SRG-OS-000063-GPOS-00032</t>
         </is>
       </c>
-      <c r="D150" s="2" t="inlineStr"/>
+      <c r="D150" s="2" t="inlineStr">
+        <is>
+          <t>CCE-89284-4</t>
+        </is>
+      </c>
       <c r="E150" s="2" t="inlineStr">
         <is>
           <t>The operating system must allow only the ISSM (or individuals or roles appointed by the ISSM) to select which auditable events are to be audited.</t>
@@ -11220,7 +11544,7 @@
       </c>
       <c r="F154" s="2" t="inlineStr">
         <is>
-          <t>The operating system must require users to re-authenticate when changing roles.</t>
+          <t>Red Hat Enterprise Linux 9 must require users to re-authenticate when changing roles.</t>
         </is>
       </c>
       <c r="G154" s="2" t="inlineStr">
@@ -11276,7 +11600,7 @@
       </c>
       <c r="F155" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement cryptographic mechanisms to protect the confidentiality of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must implement cryptographic mechanisms to protect the confidentiality of nonlocal maintenance and diagnostic communications, when used for nonlocal maintenance sessions.</t>
         </is>
       </c>
       <c r="G155" s="2" t="inlineStr">
@@ -11334,7 +11658,7 @@
       </c>
       <c r="F156" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit information from unauthorized modification.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit information from unauthorized modification.</t>
         </is>
       </c>
       <c r="G156" s="2" t="inlineStr">
@@ -11370,7 +11694,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-12 a,AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -11383,7 +11707,11 @@
           <t>SRG-OS-000037-GPOS-00015,SRG-OS-000042-GPOS-00020,SRG-OS-000062-GPOS-00031,SRG-OS-000392-GPOS-00172,SRG-OS-000462-GPOS-00206,SRG-OS-000468-GPOS-00212,SRG-OS-000471-GPOS-00215,SRG-OS-000463-GPOS-00207,SRG-OS-000465-GPOS-00209</t>
         </is>
       </c>
-      <c r="D157" s="2" t="inlineStr"/>
+      <c r="D157" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83748-4</t>
+        </is>
+      </c>
       <c r="E157" s="2" t="inlineStr">
         <is>
           <t>The operating system must generate audit records when successful/unsuccessful attempts to modify categories of information (e.g., classification levels) occur.</t>
@@ -11391,7 +11719,7 @@
       </c>
       <c r="F157" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records when successful/unsuccessful attempts to modify categories of information (e.g., classification levels) occur.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records when successful/unsuccessful attempts to modify categories of information (e.g., classification levels) occur.</t>
         </is>
       </c>
       <c r="G157" s="2" t="inlineStr">
@@ -11467,7 +11795,7 @@
       </c>
       <c r="F158" s="2" t="inlineStr">
         <is>
-          <t>The operating system must electronically verify Personal Identity Verification (PIV) credentials.</t>
+          <t>Red Hat Enterprise Linux 9 must electronically verify Personal Identity Verification (PIV) credentials.</t>
         </is>
       </c>
       <c r="G158" s="2" t="inlineStr">
@@ -11515,7 +11843,11 @@
           <t>SRG-OS-000423-GPOS-00187,SRG-OS-000033-GPOS-00014</t>
         </is>
       </c>
-      <c r="D159" s="2" t="inlineStr"/>
+      <c r="D159" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87522-9</t>
+        </is>
+      </c>
       <c r="E159" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement DoD-approved encryption to protect the confidentiality of remote access sessions.</t>
@@ -11523,7 +11855,7 @@
       </c>
       <c r="F159" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement DoD-approved encryption to protect the confidentiality of remote access sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must implement DoD-approved encryption to protect the confidentiality of remote access sessions.</t>
         </is>
       </c>
       <c r="G159" s="2" t="inlineStr">
@@ -11663,7 +11995,11 @@
           <t>SRG-OS-000445-GPOS-00199</t>
         </is>
       </c>
-      <c r="D161" s="2" t="inlineStr"/>
+      <c r="D161" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84074-4</t>
+        </is>
+      </c>
       <c r="E161" s="2" t="inlineStr">
         <is>
           <t>The operating system must verify correct operation of all security functions.</t>
@@ -11752,7 +12088,7 @@
       </c>
       <c r="F162" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect the confidentiality and integrity of communications with wireless peripherals.</t>
+          <t>Red Hat Enterprise Linux 9 must protect the confidentiality and integrity of communications with wireless peripherals.</t>
         </is>
       </c>
       <c r="G162" s="2" t="inlineStr">
@@ -11809,7 +12145,7 @@
       </c>
       <c r="F163" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all activities performed during nonlocal maintenance and diagnostic sessions.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all activities performed during nonlocal maintenance and diagnostic sessions.</t>
         </is>
       </c>
       <c r="G163" s="2" t="inlineStr">
@@ -11867,7 +12203,7 @@
       </c>
       <c r="F164" s="2" t="inlineStr">
         <is>
-          <t>The operating system must terminate all sessions and network connections related to nonlocal maintenance when nonlocal maintenance is completed.</t>
+          <t>Red Hat Enterprise Linux 9 must terminate all sessions and network connections related to nonlocal maintenance when nonlocal maintenance is completed.</t>
         </is>
       </c>
       <c r="G164" s="2" t="inlineStr">
@@ -11980,7 +12316,7 @@
       </c>
       <c r="F166" s="2" t="inlineStr">
         <is>
-          <t>The operating system must maintain the confidentiality and integrity of information during preparation for transmission.</t>
+          <t>Red Hat Enterprise Linux 9 must maintain the confidentiality and integrity of information during preparation for transmission.</t>
         </is>
       </c>
       <c r="G166" s="2" t="inlineStr">
@@ -12037,7 +12373,7 @@
       </c>
       <c r="F167" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce password complexity by requiring that at least one upper-case character be used.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce password complexity by requiring that at least one upper-case character be used.</t>
         </is>
       </c>
       <c r="G167" s="2" t="inlineStr">
@@ -12093,7 +12429,7 @@
       </c>
       <c r="F168" s="2" t="inlineStr">
         <is>
-          <t>The operating system must automatically lock an account until the locked account is released by an administrator when three unsuccessful logon attempts in 15 minutes occur.</t>
+          <t>Red Hat Enterprise Linux 9 must automatically lock an account until the locked account is released by an administrator when three unsuccessful logon attempts in 15 minutes occur.</t>
         </is>
       </c>
       <c r="G168" s="2" t="inlineStr">
@@ -12148,7 +12484,7 @@
       </c>
       <c r="F169" s="2" t="inlineStr">
         <is>
-          <t>The operating system must record time stamps for audit records that can be mapped to Coordinated Universal Time (UTC) or Greenwich Mean Time (GMT).</t>
+          <t>Red Hat Enterprise Linux 9 must record time stamps for audit records that can be mapped to Coordinated Universal Time (UTC) or Greenwich Mean Time (GMT).</t>
         </is>
       </c>
       <c r="G169" s="2" t="inlineStr">
@@ -12196,7 +12532,11 @@
           <t>SRG-OS-000480-GPOS-00225</t>
         </is>
       </c>
-      <c r="D170" s="2" t="inlineStr"/>
+      <c r="D170" s="2" t="inlineStr">
+        <is>
+          <t>CCE-88413-0</t>
+        </is>
+      </c>
       <c r="E170" s="2" t="inlineStr">
         <is>
           <t>The operating system must prevent the use of dictionary words for passwords.</t>
@@ -12204,7 +12544,7 @@
       </c>
       <c r="F170" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prevent the use of dictionary words for passwords.</t>
+          <t>Red Hat Enterprise Linux 9 must prevent the use of dictionary words for passwords.</t>
         </is>
       </c>
       <c r="G170" s="2" t="inlineStr">
@@ -12277,7 +12617,7 @@
       </c>
       <c r="F171" s="2" t="inlineStr">
         <is>
-          <t>The operating system must protect audit tools from unauthorized access.</t>
+          <t>Red Hat Enterprise Linux 9 must protect audit tools from unauthorized access.</t>
         </is>
       </c>
       <c r="G171" s="2" t="inlineStr">
@@ -12392,7 +12732,7 @@
       </c>
       <c r="F173" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records for privileged activities or other system-level access.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records for privileged activities or other system-level access.</t>
         </is>
       </c>
       <c r="G173" s="2" t="inlineStr">
@@ -12448,7 +12788,7 @@
       </c>
       <c r="F174" s="2" t="inlineStr">
         <is>
-          <t>The operating system must shut down the information system, restart the information system, and/or notify the system administrator when anomalies in the operation of any security functions are discovered.</t>
+          <t>Red Hat Enterprise Linux 9 must shut down the information system, restart the information system, and/or notify the system administrator when anomalies in the operation of any security functions are discovered.</t>
         </is>
       </c>
       <c r="G174" s="2" t="inlineStr">
@@ -12498,7 +12838,11 @@
           <t>SRG-OS-000433-GPOS-00193,SRG-OS-000095-GPOS-00049</t>
         </is>
       </c>
-      <c r="D175" s="2" t="inlineStr"/>
+      <c r="D175" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83843-3</t>
+        </is>
+      </c>
       <c r="E175" s="2" t="inlineStr">
         <is>
           <t>The operating system must implement address space layout randomization to protect its memory from unauthorized code execution.</t>
@@ -12506,7 +12850,7 @@
       </c>
       <c r="F175" s="2" t="inlineStr">
         <is>
-          <t>The operating system must implement address space layout randomization to protect its memory from unauthorized code execution.</t>
+          <t>Red Hat Enterprise Linux 9 must implement address space layout randomization to protect its memory from unauthorized code execution.</t>
         </is>
       </c>
       <c r="G175" s="2" t="inlineStr">
@@ -12585,7 +12929,7 @@
       </c>
       <c r="F176" s="2" t="inlineStr">
         <is>
-          <t>The operating system must, for networked systems, compare internal information system clocks at least every 24 hours with a server which is synchronized to one of the redundant United States Naval Observatory (USNO) time servers, or a time server designat</t>
+          <t>Red Hat Enterprise Linux 9 must, for networked systems, compare internal information system clocks at least every 24 hours with a server which is synchronized to one of the redundant United States Naval Observatory (USNO) time servers, or a time server designat</t>
         </is>
       </c>
       <c r="G176" s="2" t="inlineStr">
@@ -12634,7 +12978,11 @@
           <t>SRG-OS-000383-GPOS-00166</t>
         </is>
       </c>
-      <c r="D177" s="2" t="inlineStr"/>
+      <c r="D177" s="2" t="inlineStr">
+        <is>
+          <t>CCE-87996-5</t>
+        </is>
+      </c>
       <c r="E177" s="2" t="inlineStr">
         <is>
           <t>The operating system must prohibit the use of cached authenticators after one day.</t>
@@ -12642,7 +12990,7 @@
       </c>
       <c r="F177" s="2" t="inlineStr">
         <is>
-          <t>The operating system must prohibit the use of cached authenticators after one day.</t>
+          <t>Red Hat Enterprise Linux 9 must prohibit the use of cached authenticators after one day.</t>
         </is>
       </c>
       <c r="G177" s="2" t="inlineStr">
@@ -12710,7 +13058,7 @@
       </c>
       <c r="F178" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit all account modifications.</t>
+          <t>Red Hat Enterprise Linux 9 must audit all account modifications.</t>
         </is>
       </c>
       <c r="G178" s="2" t="inlineStr">
@@ -12822,7 +13170,7 @@
       </c>
       <c r="F180" s="2" t="inlineStr">
         <is>
-          <t>The operating system must generate audit records for all account creations, modifications, disabling, and termination events.</t>
+          <t>Red Hat Enterprise Linux 9 must generate audit records for all account creations, modifications, disabling, and termination events.</t>
         </is>
       </c>
       <c r="G180" s="2" t="inlineStr">
@@ -12870,7 +13218,11 @@
           <t>SRG-OS-000480-GPOS-00227,SRG-OS-000134-GPOS-00068</t>
         </is>
       </c>
-      <c r="D181" s="2" t="inlineStr"/>
+      <c r="D181" s="2" t="inlineStr">
+        <is>
+          <t>CCE-83842-5</t>
+        </is>
+      </c>
       <c r="E181" s="2" t="inlineStr">
         <is>
           <t>The operating system must isolate security functions from nonsecurity functions.</t>
@@ -13113,7 +13465,11 @@
           <t>SRG-OS-000480-GPOS-00229</t>
         </is>
       </c>
-      <c r="D184" s="2" t="inlineStr"/>
+      <c r="D184" s="2" t="inlineStr">
+        <is>
+          <t>CCE-90816-0</t>
+        </is>
+      </c>
       <c r="E184" s="2" t="inlineStr">
         <is>
           <t>The operating system must not allow an unattended or automatic logon to the system.</t>
@@ -13187,7 +13543,11 @@
           <t>SRG-OS-000480-GPOS-00227</t>
         </is>
       </c>
-      <c r="D185" s="2" t="inlineStr"/>
+      <c r="D185" s="2" t="inlineStr">
+        <is>
+          <t>CCE-84232-8</t>
+        </is>
+      </c>
       <c r="E185" s="2" t="inlineStr">
         <is>
           <t>The operating system must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
@@ -13195,7 +13555,7 @@
       </c>
       <c r="F185" s="2" t="inlineStr">
         <is>
-          <t>The operating system must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
+          <t>Red Hat Enterprise Linux 9 must be configured in accordance with the security configuration settings based on DoD security configuration or implementation guidance, including STIGs, NSA configuration guides, CTOs, and DTMs.</t>
         </is>
       </c>
       <c r="G185" s="2" t="inlineStr">
@@ -13360,7 +13720,7 @@
       </c>
       <c r="F187" s="2" t="inlineStr">
         <is>
-          <t>The operating system must enforce a minimum 15-character password length.</t>
+          <t>Red Hat Enterprise Linux 9 must enforce a minimum 15-character password length.</t>
         </is>
       </c>
       <c r="G187" s="2" t="inlineStr">
@@ -13487,7 +13847,7 @@
       </c>
       <c r="F189" s="2" t="inlineStr">
         <is>
-          <t>The operating system must audit the enforcement actions used to restrict access associated with changes to the system.</t>
+          <t>Red Hat Enterprise Linux 9 must audit the enforcement actions used to restrict access associated with changes to the system.</t>
         </is>
       </c>
       <c r="G189" s="2" t="inlineStr">
@@ -13543,7 +13903,7 @@
       </c>
       <c r="F190" s="2" t="inlineStr">
         <is>
-          <t>The operating system must notify designated personnel if baseline configurations are changed in an unauthorized manner.</t>
+          <t>Red Hat Enterprise Linux 9 must notify designated personnel if baseline configurations are changed in an unauthorized manner.</t>
         </is>
       </c>
       <c r="G190" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ vojtapolasek/content@08436ce586a70cfaaa22411167d9cdf80fdcb182 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>SC-5,CM-6 b,SC-5 (2)</t>
+          <t>SC-5 (2),SC-5,CM-6 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),AC-6 (8),CM-5 (1),AU-8 b,AC-6 (9),AU-7 a,AU-7 b</t>
+          <t>AU-8 b,AC-6 (9),AU-7 a,AC-6 (8),AU-7 b,CM-5 (1),AU-12 (3)</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -804,7 +804,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),AC-17 (9),CM-6 b,CM-7 b</t>
+          <t>AC-17 (1),CM-7 b,AC-17 (9),CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1175,7 +1175,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1636,7 +1636,7 @@
     <row r="16" ht="130" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
@@ -1712,7 +1712,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1843,7 +1843,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (b),IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1999,7 +1999,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MA-4 e,AC-12,MA-4 (7),SC-10</t>
+          <t>MA-4 (7),MA-4 e,SC-10,AC-12</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2074,7 +2074,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),CM-5 (1),CM-6 b,AU-7 (1),AU-14 (1),AU-12 a,AU-3,AU-7 a,AU-6 (4)</t>
+          <t>AU-7 (1),AU-7 a,CM-5 (1),AU-3,AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-12 a,CM-6 b,AU-6 (4)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2311,7 +2311,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2585,7 +2585,7 @@
     <row r="29" ht="130" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8 (2),SC-8</t>
+          <t>SC-8 (1),SC-8,SC-8 (2)</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
@@ -2714,7 +2714,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -3485,7 +3485,7 @@
     <row r="42" ht="130" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
@@ -4282,7 +4282,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),SC-13</t>
+          <t>SC-13,MA-4 (6)</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4997,7 +4997,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 (1)</t>
+          <t>AU-5 (1),AU-5 a</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5152,7 +5152,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5296,7 +5296,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5426,7 +5426,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 (3),CM-5 (1),CM-6 b,AU-8 b,AU-12 c,AU-12 a,AU-7 a,AU-7 b</t>
+          <t>AU-8 b,AU-7 a,AU-7 b,CM-5 (1),AU-12 a,AU-12 (3),CM-6 b,AU-12 c</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5983,7 +5983,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AC-2 (4),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6231,7 +6231,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (1),IA-2 (4),IA-2 (3)</t>
+          <t>IA-2 (1),IA-2 (4),IA-2 (3),IA-2 (2)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6655,7 +6655,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6809,7 +6809,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 c,AC-6 (9),AC-2 (4)</t>
+          <t>AC-2 (4),CM-5 (1),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6876,7 +6876,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2,IA-2 (4),IA-2 (2),IA-2 (3),IA-2 (5)</t>
+          <t>IA-2 (3),IA-2,IA-2 (4),IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7426,7 +7426,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8,AC-18 (1)</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7889,7 +7889,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -9033,7 +9033,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9405,7 +9405,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -10246,7 +10246,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 (1)</t>
+          <t>AC-11 (1),AC-11 b</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -10471,7 +10471,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
+          <t>SI-6 b,CM-3 (5),SI-6 d</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11125,7 +11125,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-14 (1),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11694,7 +11694,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c,AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ vojtapolasek/content@c54fccdd12390e7dca04bbef754eeb952008ed81 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -541,7 +541,7 @@
     <row r="2" ht="130" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-4</t>
+          <t>AU-4,AU-4 (1)</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="3" ht="130" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>SC-5 (2),SC-5,CM-6 b</t>
+          <t>SC-5,SC-5 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="4" ht="130" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AC-6 (9),AU-7 a,AC-6 (8),AU-7 b,CM-5 (1),AU-12 (3)</t>
+          <t>AU-8 b,AC-6 (9),CM-5 (1),AU-7 b,AC-6 (8),AU-12 (3),AU-7 a</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -804,7 +804,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b,AC-17 (9),CM-6 b</t>
+          <t>CM-7 b,AC-17 (1),AC-17 (9),CM-6 b</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1024,7 +1024,7 @@
     <row r="8" ht="130" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -1175,7 +1175,7 @@
     <row r="10" ht="130" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (5) (b),CM-7 (2)</t>
+          <t>CM-7 (2),CM-7 (5) (b)</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -1558,7 +1558,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),IA-8,IA-2</t>
+          <t>IA-2,AU-3 (1),IA-8</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -1699,7 +1699,12 @@
         </is>
       </c>
       <c r="L16" s="2" t="n"/>
-      <c r="M16" s="2" t="inlineStr"/>
+      <c r="M16" s="2" t="inlineStr">
+        <is>
+          <t>Edit "/etc/systemd/system.conf" and add or edit the following line:
+CtrlAltDelBurstAction=none</t>
+        </is>
+      </c>
       <c r="N16" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -1712,7 +1717,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -1843,7 +1848,7 @@
     <row r="19" ht="130" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
@@ -1999,7 +2004,7 @@
     <row r="21" ht="130" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),MA-4 e,SC-10,AC-12</t>
+          <t>SC-10,MA-4 e,MA-4 (7),AC-12</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
@@ -2074,7 +2079,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>AU-7 (1),AU-7 a,CM-5 (1),AU-3,AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-12 a,CM-6 b,AU-6 (4)</t>
+          <t>AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-7 (1),AU-3,CM-5 (1),AU-6 (4),CM-6 b,AU-7 a,AU-12 a</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2311,7 +2316,7 @@
     <row r="25" ht="130" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
@@ -2714,7 +2719,7 @@
     <row r="31" ht="130" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
@@ -2926,7 +2931,7 @@
     <row r="34" ht="130" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-11 a</t>
+          <t>AC-11 a,AC-11 b</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
@@ -3210,7 +3215,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AU-9,SI-11 b</t>
+          <t>SI-11 b,AU-9</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3625,14 +3630,20 @@
         <is>
           <t>Run the following command to ensure the "maxlogins" value is
 configured for all users on the system:
- # grep "maxlogins" /etc/security/limits.conf 
+ # grep "maxlogins" /etc/security/limits.conf /etc/security/limits.d/*.conf 
 You should receive output similar to the following:
- *\t\thard\tmaxlogins\t 
+ *\t\thard\tmaxlogins\t10 
 If maxlogins is not equal to or less than the expected value then this is a finding.</t>
         </is>
       </c>
       <c r="L43" s="2" t="n"/>
-      <c r="M43" s="2" t="inlineStr"/>
+      <c r="M43" s="2" t="inlineStr">
+        <is>
+          <t>Configure the operating system to limit the number of concurrent sessions to "10" for all accounts and/or account types.
+Add the following line to the top of the /etc/security/limits.conf or in a ".conf" file defined in /etc/security/limits.d/ :
+* hard maxlogins 10</t>
+        </is>
+      </c>
       <c r="N43" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -3719,7 +3730,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 b,AC-8 a</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a,AC-8 b</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -4066,7 +4077,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (5)</t>
+          <t>IA-2 (5),CM-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4498,7 +4509,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4997,7 +5008,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-5 (1),AU-5 a</t>
+          <t>AU-5 a,AU-5 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5152,7 +5163,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5296,7 +5307,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5426,7 +5437,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-7 a,AU-7 b,CM-5 (1),AU-12 a,AU-12 (3),CM-6 b,AU-12 c</t>
+          <t>AU-8 b,AU-12 c,CM-5 (1),AU-7 b,CM-6 b,AU-12 (3),AU-7 a,AU-12 a</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5983,7 +5994,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AC-2 (4),AU-3 (1),MA-4 (1) (a),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AC-2 (4),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6156,7 +6167,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6231,7 +6242,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (1),IA-2 (4),IA-2 (3),IA-2 (2)</t>
+          <t>IA-2 (4),IA-2 (2),IA-2 (3),IA-2 (1)</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6655,7 +6666,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -6809,7 +6820,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),CM-5 (1),AC-6 (9),AU-12 c</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9),CM-5 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -6876,7 +6887,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (3),IA-2,IA-2 (4),IA-2 (2),IA-2 (5)</t>
+          <t>IA-2 (4),IA-2 (2),IA-2 (3),IA-2,IA-2 (5)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -6960,7 +6971,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7040,7 +7051,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7506,7 +7517,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 (1) (a),AU-8 b</t>
+          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7562,15 +7573,21 @@
       </c>
       <c r="K97" s="2" t="inlineStr">
         <is>
-          <t>To verify that "maxpoll" has been set properly, perform the following:
+          <t>Verify Red Hat Enterprise Linux 9 is securely comparing internal information system clocks at a regular interval with an NTP server with the following commands:
+To verify that "maxpoll" has been set properly, perform the following:
  $ sudo grep maxpoll /etc/ntp.conf /etc/chrony.conf 
 The output should return:
- maxpoll  .
-If it does not exist or maxpoll has not been set to the expected value then this is a finding.</t>
+ maxpoll 16 .
+If maxpoll does not exist or maxpoll has not been set to the expected value of 16 then this is a finding.</t>
         </is>
       </c>
       <c r="L97" s="2" t="n"/>
-      <c r="M97" s="2" t="inlineStr"/>
+      <c r="M97" s="2" t="inlineStr">
+        <is>
+          <t>Configure Red Hat Enterprise Linux 9 to securely compare internal information system clocks at a regular interval with an NTP server by adding/modifying the following line in the /etc/chrony.conf file.
+server [ntp.server.name] iburst maxpoll 16</t>
+        </is>
+      </c>
       <c r="N97" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -7815,7 +7832,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -7889,7 +7906,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8483,7 +8500,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-5 b,AU-5 a</t>
+          <t>AU-5 a,AU-5 b</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9033,7 +9050,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9405,7 +9422,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -9668,7 +9685,7 @@
     <row r="128" ht="130" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b,CM-7 a</t>
+          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
         </is>
       </c>
       <c r="B128" s="2" t="inlineStr">
@@ -10471,7 +10488,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,CM-3 (5),SI-6 d</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11125,7 +11142,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-3,AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>AU-14 (1),MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11694,7 +11711,7 @@
     <row r="157" ht="130" customHeight="1">
       <c r="A157" s="2" t="inlineStr">
         <is>
-          <t>AU-3,MA-4 (1) (a),AU-3 (1),AU-12 a,AU-12 c</t>
+          <t>MA-4 (1) (a),AU-3 (1),AU-3,AU-12 c,AU-12 a</t>
         </is>
       </c>
       <c r="B157" s="2" t="inlineStr">
@@ -12825,7 +12842,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -13024,7 +13041,13 @@
         </is>
       </c>
       <c r="L177" s="2" t="n"/>
-      <c r="M177" s="2" t="inlineStr"/>
+      <c r="M177" s="2" t="inlineStr">
+        <is>
+          <t>Configure the SSSD to prohibit the use of cached authentications after one day.
+Add or change the following line in "/etc/sssd/sssd.conf" just below the line "[pam]".
+offline_credentials_expiration = 1</t>
+        </is>
+      </c>
       <c r="N177" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ vojtapolasek/content@5283c0baed996e97326890b8fc55822a76bbd8ce 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -784,7 +784,7 @@
     <row r="5" ht="130" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>SC-5,CM-6 b,SC-5 (2)</t>
+          <t>CM-6 b,SC-5,SC-5 (2)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="6" ht="130" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>AU-8 b,AU-7 a,AC-6 (9),AC-6 (8),CM-5 (1),AU-7 b,AU-12 (3)</t>
+          <t>AU-12 (3),AU-7 b,AC-6 (9),AU-8 b,CM-5 (1),AC-6 (8),AU-7 a</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -893,7 +893,7 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>SRG-OS-000326-GPOS-00126,SRG-OS-000327-GPOS-00127,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000359-GPOS-00146,SRG-OS-000365-GPOS-00152</t>
+          <t>SRG-OS-000326-GPOS-00126,SRG-OS-000327-GPOS-00127,SRG-OS-000337-GPOS-00129,SRG-OS-000348-GPOS-00136,SRG-OS-000349-GPOS-00137,SRG-OS-000350-GPOS-00138,SRG-OS-000351-GPOS-00139,SRG-OS-000352-GPOS-00140,SRG-OS-000353-GPOS-00141,SRG-OS-000354-GPOS-00142,SRG-OS-000358-GPOS-00145,SRG-OS-000365-GPOS-00152</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -963,7 +963,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-8 b,AU-7 a,CM-6 b,AU-12 a,CM-5 (1),AU-7 b,AU-12 (3)</t>
+          <t>AU-12 (3),CM-6 b,AU-7 b,AU-8 b,CM-5 (1),AU-12 a,AU-7 a,AU-12 c</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1015,7 +1015,7 @@
       <c r="K7" s="2" t="inlineStr">
         <is>
           <t>Run the following command to determine if the  audit  package is installed:  $ rpm -q audit 
-If the package is not installed then this is a finding.</t>
+If the audit package is not installed then this is a finding.</t>
         </is>
       </c>
       <c r="L7" s="2" t="n"/>
@@ -1269,7 +1269,7 @@
     <row r="11" ht="130" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
@@ -1346,7 +1346,7 @@
     <row r="12" ht="130" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
@@ -1726,7 +1726,7 @@
     <row r="17" ht="130" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
@@ -2096,7 +2096,7 @@
     <row r="22" ht="130" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
@@ -2170,7 +2170,7 @@
     <row r="23" ht="130" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-6 b</t>
+          <t>CM-6 b,CM-7 (2)</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
@@ -3298,7 +3298,7 @@
     <row r="38" ht="130" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
@@ -3382,7 +3382,7 @@
     <row r="39" ht="130" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
@@ -3467,7 +3467,7 @@
     <row r="40" ht="130" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
@@ -3539,7 +3539,7 @@
     <row r="41" ht="130" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>AC-7 b,AC-7 a</t>
+          <t>AC-7 a,AC-7 b</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="45" ht="130" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
-          <t>IA-2,AU-3 (1),IA-8</t>
+          <t>IA-8,AU-3 (1),IA-2</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
@@ -3922,7 +3922,7 @@
     <row r="46" ht="130" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
@@ -3997,7 +3997,7 @@
     <row r="47" ht="130" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
@@ -4072,7 +4072,7 @@
     <row r="48" ht="130" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
@@ -4147,7 +4147,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4297,7 +4297,7 @@
     <row r="51" ht="130" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
@@ -4372,7 +4372,7 @@
     <row r="52" ht="130" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
@@ -4447,7 +4447,7 @@
     <row r="53" ht="130" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
@@ -4522,7 +4522,7 @@
     <row r="54" ht="130" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
@@ -4597,7 +4597,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4672,7 +4672,7 @@
     <row r="56" ht="130" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
@@ -4747,7 +4747,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4822,7 +4822,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4897,7 +4897,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -4977,7 +4977,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5060,7 +5060,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5140,7 +5140,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5220,7 +5220,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5300,7 +5300,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5380,7 +5380,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5454,7 +5454,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5528,7 +5528,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5602,7 +5602,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5750,7 +5750,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5823,7 +5823,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5896,7 +5896,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -6042,7 +6042,7 @@
     <row r="74" ht="130" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B74" s="2" t="inlineStr">
@@ -6115,7 +6115,7 @@
     <row r="75" ht="130" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B75" s="2" t="inlineStr">
@@ -6188,7 +6188,7 @@
     <row r="76" ht="130" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B76" s="2" t="inlineStr">
@@ -6262,7 +6262,7 @@
     <row r="77" ht="130" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B77" s="2" t="inlineStr">
@@ -6336,7 +6336,7 @@
     <row r="78" ht="130" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B78" s="2" t="inlineStr">
@@ -6410,7 +6410,7 @@
     <row r="79" ht="130" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B79" s="2" t="inlineStr">
@@ -6481,7 +6481,7 @@
     <row r="80" ht="130" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B80" s="2" t="inlineStr">
@@ -6561,7 +6561,7 @@
     <row r="81" ht="130" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
@@ -6641,7 +6641,7 @@
     <row r="82" ht="130" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B82" s="2" t="inlineStr">
@@ -6721,7 +6721,7 @@
     <row r="83" ht="130" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B83" s="2" t="inlineStr">
@@ -6801,7 +6801,7 @@
     <row r="84" ht="130" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B84" s="2" t="inlineStr">
@@ -6881,7 +6881,7 @@
     <row r="85" ht="130" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B85" s="2" t="inlineStr">
@@ -6961,7 +6961,7 @@
     <row r="86" ht="130" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B86" s="2" t="inlineStr">
@@ -7041,7 +7041,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7121,7 +7121,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7201,7 +7201,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7281,7 +7281,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7361,7 +7361,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),MA-4 (1) (a)</t>
+          <t>AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7437,7 +7437,7 @@
     <row r="92" ht="130" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B92" s="2" t="inlineStr">
@@ -7514,7 +7514,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7594,7 +7594,7 @@
     <row r="94" ht="130" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B94" s="2" t="inlineStr">
@@ -7674,7 +7674,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7754,7 +7754,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7834,7 +7834,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3 (1),AU-3</t>
+          <t>AU-3 (1),AU-3,MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -7914,7 +7914,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -7994,7 +7994,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8074,7 +8074,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8154,7 +8154,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8234,7 +8234,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8307,7 +8307,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8388,7 +8388,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8469,7 +8469,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8540,7 +8540,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8615,7 +8615,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8697,7 +8697,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -8779,7 +8779,7 @@
     <row r="109" ht="130" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B109" s="2" t="inlineStr">
@@ -8861,7 +8861,7 @@
     <row r="110" ht="130" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B110" s="2" t="inlineStr">
@@ -8943,7 +8943,7 @@
     <row r="111" ht="130" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AC-2 (4),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-12 a,AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B111" s="2" t="inlineStr">
@@ -9025,7 +9025,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-3 (1),AU-14 (1),AU-12 a,AU-3,MA-4 (1) (a)</t>
+          <t>AU-3,AU-14 (1),AU-12 a,AU-3 (1),MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9275,7 +9275,7 @@
     <row r="115" ht="130" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
-          <t>AC-11 b,AC-6 (10)</t>
+          <t>AC-6 (10),AC-11 b</t>
         </is>
       </c>
       <c r="B115" s="2" t="inlineStr">
@@ -9719,7 +9719,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9790,7 +9790,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-12 a,MA-4 (1) (a),AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9861,7 +9861,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,AU-9</t>
+          <t>AU-9,AU-12 c</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10234,7 +10234,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>AC-2 (4),AC-6 (9),AU-12 c,CM-5 (1)</t>
+          <t>CM-5 (1),AC-2 (4),AC-6 (9),AU-12 c</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -10357,7 +10357,7 @@
     <row r="129" ht="130" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b,IA-5 (1) (b)</t>
+          <t>CM-6 b,IA-5 (1) (a),IA-5 (1) (b)</t>
         </is>
       </c>
       <c r="B129" s="2" t="inlineStr">
@@ -10677,7 +10677,7 @@
     <row r="133" ht="130" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 c,AC-17 (2),SC-8</t>
+          <t>AC-17 (2),SC-13,MA-4 c,SC-8</t>
         </is>
       </c>
       <c r="B133" s="2" t="inlineStr">
@@ -10759,7 +10759,7 @@
     <row r="134" ht="130" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (7),SC-10,AC-12,MA-4 e</t>
+          <t>MA-4 (7),SC-10,MA-4 e,AC-12</t>
         </is>
       </c>
       <c r="B134" s="2" t="inlineStr">
@@ -10834,7 +10834,7 @@
     <row r="135" ht="130" customHeight="1">
       <c r="A135" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B135" s="2" t="inlineStr">
@@ -10913,7 +10913,7 @@
     <row r="136" ht="130" customHeight="1">
       <c r="A136" s="2" t="inlineStr">
         <is>
-          <t>AC-12,SC-10</t>
+          <t>SC-10,AC-12</t>
         </is>
       </c>
       <c r="B136" s="2" t="inlineStr">
@@ -11066,7 +11066,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>AU-7 (1),AU-7 a,AU-3 (1),CM-6 b,AU-6 (4),AU-14 (1),CM-5 (1),AU-12 a,MA-4 (1) (a),AU-3</t>
+          <t>AU-3,AU-6 (4),CM-6 b,AU-14 (1),CM-5 (1),AU-12 a,AU-3 (1),AU-7 a,MA-4 (1) (a),AU-7 (1)</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11468,7 +11468,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11537,7 +11537,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11606,7 +11606,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11676,7 +11676,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -11745,7 +11745,7 @@
     <row r="147" ht="130" customHeight="1">
       <c r="A147" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B147" s="2" t="inlineStr">
@@ -11814,7 +11814,7 @@
     <row r="148" ht="130" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B148" s="2" t="inlineStr">
@@ -11884,7 +11884,7 @@
     <row r="149" ht="130" customHeight="1">
       <c r="A149" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B149" s="2" t="inlineStr">
@@ -11953,7 +11953,7 @@
     <row r="150" ht="130" customHeight="1">
       <c r="A150" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B150" s="2" t="inlineStr">
@@ -12022,7 +12022,7 @@
     <row r="151" ht="130" customHeight="1">
       <c r="A151" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B151" s="2" t="inlineStr">
@@ -12092,7 +12092,7 @@
     <row r="152" ht="130" customHeight="1">
       <c r="A152" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B152" s="2" t="inlineStr">
@@ -12161,7 +12161,7 @@
     <row r="153" ht="130" customHeight="1">
       <c r="A153" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B153" s="2" t="inlineStr">
@@ -12230,7 +12230,7 @@
     <row r="154" ht="130" customHeight="1">
       <c r="A154" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B154" s="2" t="inlineStr">
@@ -12299,7 +12299,7 @@
     <row r="155" ht="130" customHeight="1">
       <c r="A155" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B155" s="2" t="inlineStr">
@@ -13137,7 +13137,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (2),SC-8,SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13369,7 +13369,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -14134,7 +14134,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-6 (4),AU-4 (1)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14205,7 +14205,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b,AC-17 (9),CM-6 b</t>
+          <t>CM-7 b,AC-17 (9),AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14282,7 +14282,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b,CM-6 b</t>
+          <t>CM-7 b,CM-6 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -15682,7 +15682,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16197,7 +16197,7 @@
     <row r="207" ht="130" customHeight="1">
       <c r="A207" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),CM-6 b</t>
+          <t>CM-6 b,AU-4 (1)</t>
         </is>
       </c>
       <c r="B207" s="2" t="inlineStr">
@@ -16277,7 +16277,7 @@
     <row r="208" ht="130" customHeight="1">
       <c r="A208" s="2" t="inlineStr">
         <is>
-          <t>SC-28,SC-28 (1)</t>
+          <t>SC-28 (1),SC-28</t>
         </is>
       </c>
       <c r="B208" s="2" t="inlineStr">
@@ -17465,7 +17465,7 @@
     <row r="221" ht="130" customHeight="1">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (5),CM-6 b</t>
+          <t>CM-6 b,IA-2 (5)</t>
         </is>
       </c>
       <c r="B221" s="2" t="inlineStr">
@@ -17543,7 +17543,7 @@
     <row r="222" ht="130" customHeight="1">
       <c r="A222" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2 (4),IA-2,IA-2 (5)</t>
+          <t>IA-2,IA-2 (3),IA-2 (4),IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B222" s="2" t="inlineStr">
@@ -17628,7 +17628,7 @@
     <row r="223" ht="130" customHeight="1">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),IA-2 (3),IA-2 (4),IA-2,IA-2 (5)</t>
+          <t>IA-2,IA-2 (3),IA-2 (4),IA-2 (2),IA-2 (5)</t>
         </is>
       </c>
       <c r="B223" s="2" t="inlineStr">
@@ -17713,7 +17713,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>SC-8 (1),SC-8,AC-18 (1)</t>
+          <t>AC-18 (1),SC-8,SC-8 (1)</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17880,7 +17880,7 @@
     <row r="226" ht="130" customHeight="1">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),IA-7</t>
+          <t>IA-7,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B226" s="2" t="inlineStr">
@@ -17963,7 +17963,7 @@
     <row r="227" ht="130" customHeight="1">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B227" s="2" t="inlineStr">
@@ -18039,7 +18039,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18124,7 +18124,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-6 b</t>
+          <t>CM-6 b,IA-7</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -18281,7 +18281,7 @@
     <row r="231" ht="130" customHeight="1">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B231" s="2" t="inlineStr">
@@ -18444,7 +18444,7 @@
     <row r="233" ht="130" customHeight="1">
       <c r="A233" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (6),AC-17 (2)</t>
+          <t>AC-17 (2),MA-4 (6)</t>
         </is>
       </c>
       <c r="B233" s="2" t="inlineStr">
@@ -19116,7 +19116,7 @@
     <row r="242" ht="130" customHeight="1">
       <c r="A242" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B242" s="2" t="inlineStr">
@@ -19187,7 +19187,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -19349,7 +19349,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2,SI-16</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -19509,7 +19509,7 @@
     <row r="247" ht="130" customHeight="1">
       <c r="A247" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B247" s="2" t="inlineStr">
@@ -20423,7 +20423,7 @@
     <row r="259" ht="130" customHeight="1">
       <c r="A259" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B259" s="2" t="inlineStr">
@@ -20498,7 +20498,7 @@
     <row r="260" ht="130" customHeight="1">
       <c r="A260" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B260" s="2" t="inlineStr">
@@ -20586,7 +20586,7 @@
     <row r="261" ht="130" customHeight="1">
       <c r="A261" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B261" s="2" t="inlineStr">
@@ -20663,7 +20663,7 @@
     <row r="262" ht="130" customHeight="1">
       <c r="A262" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-6 b</t>
+          <t>CM-6 b,IA-3</t>
         </is>
       </c>
       <c r="B262" s="2" t="inlineStr">
@@ -21261,7 +21261,7 @@
     <row r="270" ht="130" customHeight="1">
       <c r="A270" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (2),CM-6 b</t>
+          <t>CM-6 b,IA-2 (2)</t>
         </is>
       </c>
       <c r="B270" s="2" t="inlineStr">
@@ -21348,7 +21348,7 @@
     <row r="271" ht="130" customHeight="1">
       <c r="A271" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (3),IA-2 (1),IA-2 (2)</t>
+          <t>IA-2 (1),IA-2 (3),IA-2 (4),IA-2 (2)</t>
         </is>
       </c>
       <c r="B271" s="2" t="inlineStr">
@@ -21517,7 +21517,7 @@
     <row r="273" ht="130" customHeight="1">
       <c r="A273" s="2" t="inlineStr">
         <is>
-          <t>AU-12 c,MA-4 (1) (a)</t>
+          <t>MA-4 (1) (a),AU-12 c</t>
         </is>
       </c>
       <c r="B273" s="2" t="inlineStr">
@@ -21816,7 +21816,7 @@
     <row r="277" ht="130" customHeight="1">
       <c r="A277" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B277" s="2" t="inlineStr">
@@ -21904,7 +21904,7 @@
     <row r="278" ht="130" customHeight="1">
       <c r="A278" s="2" t="inlineStr">
         <is>
-          <t>SC-2,SC-4</t>
+          <t>SC-4,SC-2</t>
         </is>
       </c>
       <c r="B278" s="2" t="inlineStr">
@@ -22142,7 +22142,7 @@
     <row r="281" ht="130" customHeight="1">
       <c r="A281" s="2" t="inlineStr">
         <is>
-          <t>AU-12 a,CM-6 b</t>
+          <t>CM-6 b,AU-12 a</t>
         </is>
       </c>
       <c r="B281" s="2" t="inlineStr">
@@ -23465,7 +23465,7 @@
     <row r="298" ht="130" customHeight="1">
       <c r="A298" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (11)</t>
+          <t>IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B298" s="2" t="inlineStr">
@@ -23634,7 +23634,7 @@
     <row r="300" ht="130" customHeight="1">
       <c r="A300" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (12),IA-2 (1),IA-2 (11)</t>
+          <t>IA-2 (1),IA-2 (11),IA-2 (12)</t>
         </is>
       </c>
       <c r="B300" s="2" t="inlineStr">
@@ -24456,7 +24456,7 @@
     <row r="310" ht="130" customHeight="1">
       <c r="A310" s="2" t="inlineStr">
         <is>
-          <t>AU-8 (1) (b),AU-8 b,AU-8 (1) (a)</t>
+          <t>AU-8 b,AU-8 (1) (b),AU-8 (1) (a)</t>
         </is>
       </c>
       <c r="B310" s="2" t="inlineStr">
@@ -25409,7 +25409,7 @@
     <row r="322" ht="130" customHeight="1">
       <c r="A322" s="2" t="inlineStr">
         <is>
-          <t>IA-11,AC-3 (4)</t>
+          <t>AC-3 (4),IA-11</t>
         </is>
       </c>
       <c r="B322" s="2" t="inlineStr">
@@ -27172,7 +27172,7 @@
     <row r="345" ht="130" customHeight="1">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B345" s="2" t="inlineStr">
@@ -27335,7 +27335,7 @@
     <row r="347" ht="130" customHeight="1">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-7 a,CM-6 b</t>
+          <t>CM-7 a,CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B347" s="2" t="inlineStr">
@@ -28180,7 +28180,7 @@
     <row r="358" ht="130" customHeight="1">
       <c r="A358" s="2" t="inlineStr">
         <is>
-          <t>AC-11 (1),AC-11 b</t>
+          <t>AC-11 b,AC-11 (1)</t>
         </is>
       </c>
       <c r="B358" s="2" t="inlineStr">
@@ -28429,7 +28429,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>SI-6 d,CM-3 (5),SI-6 b</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -28900,7 +28900,7 @@
     <row r="367" ht="130" customHeight="1">
       <c r="A367" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-7 a</t>
+          <t>CM-7 a,SI-16</t>
         </is>
       </c>
       <c r="B367" s="2" t="inlineStr">
@@ -30343,7 +30343,7 @@
     <row r="385" ht="130" customHeight="1">
       <c r="A385" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (2),CM-6 b</t>
+          <t>CM-6 b,AC-17 (2)</t>
         </is>
       </c>
       <c r="B385" s="2" t="inlineStr">
@@ -30791,7 +30791,7 @@
     <row r="391" ht="130" customHeight="1">
       <c r="A391" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (a),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B391" s="2" t="inlineStr">
@@ -31357,7 +31357,7 @@
     <row r="398" ht="130" customHeight="1">
       <c r="A398" s="2" t="inlineStr">
         <is>
-          <t>SI-16,CM-6 b</t>
+          <t>CM-6 b,SI-16</t>
         </is>
       </c>
       <c r="B398" s="2" t="inlineStr">
@@ -35193,7 +35193,7 @@
     <row r="448" ht="130" customHeight="1">
       <c r="A448" s="2" t="inlineStr">
         <is>
-          <t>IA-5 (1) (c),CM-6 b</t>
+          <t>CM-6 b,IA-5 (1) (c)</t>
         </is>
       </c>
       <c r="B448" s="2" t="inlineStr">
@@ -41227,7 +41227,7 @@
     <row r="524" ht="130" customHeight="1">
       <c r="A524" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B524" s="2" t="inlineStr">
@@ -41314,7 +41314,7 @@
     <row r="525" ht="130" customHeight="1">
       <c r="A525" s="2" t="inlineStr">
         <is>
-          <t>SC-2,CM-6 b</t>
+          <t>CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B525" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Deploying to gh-pages from @ vojtapolasek/content@af6aa9625e2319d9f47458daf142267901ba9244 🚀
</commit_message>
<xml_diff>
--- a/srg_mapping/srg-mapping-rhel9.xlsx
+++ b/srg_mapping/srg-mapping-rhel9.xlsx
@@ -964,7 +964,7 @@
     <row r="7" ht="130" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AU-5 a,AU-5 b</t>
+          <t>AU-5 b,AU-5 a</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
@@ -1446,7 +1446,7 @@
     <row r="13" ht="130" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),CM-5 (1),CM-6 b,MA-4 (1) (a),AU-3,AU-7 (1),AU-7 a,AU-14 (1),AU-12 a,AU-6 (4)</t>
+          <t>AU-3,AU-6 (4),AU-7 (1),MA-4 (1) (a),CM-6 b,AU-12 a,CM-5 (1),AU-14 (1),AU-3 (1),AU-7 a</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
@@ -1531,7 +1531,7 @@
     <row r="14" ht="130" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -1607,7 +1607,7 @@
     <row r="15" ht="130" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>CM-7 (2),CM-7 (5) (b)</t>
+          <t>CM-7 (5) (b),CM-7 (2)</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
@@ -3249,7 +3249,7 @@
     <row r="37" ht="130" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-14 (1),AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-14 (1),AU-3 (1)</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
@@ -3782,7 +3782,7 @@
     <row r="44" ht="130" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>AU-4 (1),AU-3</t>
+          <t>AU-3,AU-4 (1)</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
@@ -4161,7 +4161,7 @@
     <row r="49" ht="130" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1),AU-6 (4)</t>
+          <t>AU-6 (4),AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
@@ -4231,7 +4231,7 @@
     <row r="50" ht="130" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-4 (1)</t>
+          <t>AU-4 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
@@ -4636,7 +4636,7 @@
     <row r="55" ht="130" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>SI-6 b,SI-6 d,CM-3 (5)</t>
+          <t>SI-6 d,SI-6 b,CM-3 (5)</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
@@ -4812,7 +4812,7 @@
     <row r="57" ht="130" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B57" s="2" t="inlineStr">
@@ -4887,7 +4887,7 @@
     <row r="58" ht="130" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B58" s="2" t="inlineStr">
@@ -4962,7 +4962,7 @@
     <row r="59" ht="130" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B59" s="2" t="inlineStr">
@@ -5037,7 +5037,7 @@
     <row r="60" ht="130" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B60" s="2" t="inlineStr">
@@ -5112,7 +5112,7 @@
     <row r="61" ht="130" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
@@ -5187,7 +5187,7 @@
     <row r="62" ht="130" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B62" s="2" t="inlineStr">
@@ -5262,7 +5262,7 @@
     <row r="63" ht="130" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B63" s="2" t="inlineStr">
@@ -5337,7 +5337,7 @@
     <row r="64" ht="130" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B64" s="2" t="inlineStr">
@@ -5412,7 +5412,7 @@
     <row r="65" ht="130" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B65" s="2" t="inlineStr">
@@ -5487,7 +5487,7 @@
     <row r="66" ht="130" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 (3),CM-6 b,AU-8 b,AU-7 a,AU-7 b,AU-12 c,AU-12 a</t>
+          <t>AU-12 a,CM-6 b,AU-12 c,CM-5 (1),AU-7 b,AU-8 b,AU-7 a,AU-12 (3)</t>
         </is>
       </c>
       <c r="B66" s="2" t="inlineStr">
@@ -5561,7 +5561,7 @@
     <row r="67" ht="130" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B67" s="2" t="inlineStr">
@@ -5642,7 +5642,7 @@
     <row r="68" ht="130" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B68" s="2" t="inlineStr">
@@ -5723,7 +5723,7 @@
     <row r="69" ht="130" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B69" s="2" t="inlineStr">
@@ -5805,7 +5805,7 @@
     <row r="70" ht="130" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B70" s="2" t="inlineStr">
@@ -5887,7 +5887,7 @@
     <row r="71" ht="130" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B71" s="2" t="inlineStr">
@@ -5969,7 +5969,7 @@
     <row r="72" ht="130" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B72" s="2" t="inlineStr">
@@ -6051,7 +6051,7 @@
     <row r="73" ht="130" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B73" s="2" t="inlineStr">
@@ -7171,7 +7171,7 @@
     <row r="87" ht="130" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B87" s="2" t="inlineStr">
@@ -7245,7 +7245,7 @@
     <row r="88" ht="130" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B88" s="2" t="inlineStr">
@@ -7319,7 +7319,7 @@
     <row r="89" ht="130" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B89" s="2" t="inlineStr">
@@ -7393,7 +7393,7 @@
     <row r="90" ht="130" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B90" s="2" t="inlineStr">
@@ -7473,7 +7473,7 @@
     <row r="91" ht="130" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B91" s="2" t="inlineStr">
@@ -7634,7 +7634,7 @@
     <row r="93" ht="130" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
-          <t>SC-13,MA-4 (6)</t>
+          <t>MA-4 (6),SC-13</t>
         </is>
       </c>
       <c r="B93" s="2" t="inlineStr">
@@ -7817,7 +7817,7 @@
     <row r="95" ht="130" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B95" s="2" t="inlineStr">
@@ -7893,7 +7893,7 @@
     <row r="96" ht="130" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-9 (3)</t>
+          <t>AU-9 (3),AU-9</t>
         </is>
       </c>
       <c r="B96" s="2" t="inlineStr">
@@ -7969,7 +7969,7 @@
     <row r="97" ht="130" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B97" s="2" t="inlineStr">
@@ -8044,7 +8044,7 @@
     <row r="98" ht="130" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B98" s="2" t="inlineStr">
@@ -8119,7 +8119,7 @@
     <row r="99" ht="130" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B99" s="2" t="inlineStr">
@@ -8194,7 +8194,7 @@
     <row r="100" ht="130" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B100" s="2" t="inlineStr">
@@ -8274,7 +8274,7 @@
     <row r="101" ht="130" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B101" s="2" t="inlineStr">
@@ -8348,7 +8348,7 @@
     <row r="102" ht="130" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B102" s="2" t="inlineStr">
@@ -8422,7 +8422,7 @@
     <row r="103" ht="130" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B103" s="2" t="inlineStr">
@@ -8496,7 +8496,7 @@
     <row r="104" ht="130" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B104" s="2" t="inlineStr">
@@ -8570,7 +8570,7 @@
     <row r="105" ht="130" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B105" s="2" t="inlineStr">
@@ -8644,7 +8644,7 @@
     <row r="106" ht="130" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B106" s="2" t="inlineStr">
@@ -8724,7 +8724,7 @@
     <row r="107" ht="130" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B107" s="2" t="inlineStr">
@@ -8804,7 +8804,7 @@
     <row r="108" ht="130" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B108" s="2" t="inlineStr">
@@ -9134,7 +9134,7 @@
     <row r="112" ht="130" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,AC-11 b</t>
+          <t>AC-11 b,AC-11 a</t>
         </is>
       </c>
       <c r="B112" s="2" t="inlineStr">
@@ -9553,7 +9553,7 @@
     <row r="117" ht="130" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2),SC-13,MA-4 c</t>
+          <t>AC-17 (2),SC-13,SC-8,MA-4 c</t>
         </is>
       </c>
       <c r="B117" s="2" t="inlineStr">
@@ -9635,7 +9635,7 @@
     <row r="118" ht="130" customHeight="1">
       <c r="A118" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B118" s="2" t="inlineStr">
@@ -9713,7 +9713,7 @@
     <row r="119" ht="130" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B119" s="2" t="inlineStr">
@@ -9791,7 +9791,7 @@
     <row r="120" ht="130" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B120" s="2" t="inlineStr">
@@ -9869,7 +9869,7 @@
     <row r="121" ht="130" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B121" s="2" t="inlineStr">
@@ -9949,7 +9949,7 @@
     <row r="122" ht="130" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B122" s="2" t="inlineStr">
@@ -10018,7 +10018,7 @@
     <row r="123" ht="130" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B123" s="2" t="inlineStr">
@@ -10087,7 +10087,7 @@
     <row r="124" ht="130" customHeight="1">
       <c r="A124" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B124" s="2" t="inlineStr">
@@ -10156,7 +10156,7 @@
     <row r="125" ht="130" customHeight="1">
       <c r="A125" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B125" s="2" t="inlineStr">
@@ -10225,7 +10225,7 @@
     <row r="126" ht="130" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B126" s="2" t="inlineStr">
@@ -10305,7 +10305,7 @@
     <row r="127" ht="130" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
         <is>
-          <t>SC-28 (1),SC-28</t>
+          <t>SC-28,SC-28 (1)</t>
         </is>
       </c>
       <c r="B127" s="2" t="inlineStr">
@@ -11072,7 +11072,7 @@
     <row r="137" ht="130" customHeight="1">
       <c r="A137" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B137" s="2" t="inlineStr">
@@ -11153,7 +11153,7 @@
     <row r="138" ht="130" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B138" s="2" t="inlineStr">
@@ -11239,7 +11239,7 @@
     <row r="139" ht="130" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-6 (10)</t>
+          <t>AC-6 (10),CM-6 b</t>
         </is>
       </c>
       <c r="B139" s="2" t="inlineStr">
@@ -11605,7 +11605,7 @@
     <row r="143" ht="130" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B143" s="2" t="inlineStr">
@@ -11685,7 +11685,7 @@
     <row r="144" ht="130" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B144" s="2" t="inlineStr">
@@ -11765,7 +11765,7 @@
     <row r="145" ht="130" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B145" s="2" t="inlineStr">
@@ -11845,7 +11845,7 @@
     <row r="146" ht="130" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B146" s="2" t="inlineStr">
@@ -12862,7 +12862,7 @@
     <row r="159" ht="130" customHeight="1">
       <c r="A159" s="2" t="inlineStr">
         <is>
-          <t>IA-7,CM-7 a</t>
+          <t>CM-7 a,IA-7</t>
         </is>
       </c>
       <c r="B159" s="2" t="inlineStr">
@@ -12941,7 +12941,7 @@
     <row r="160" ht="130" customHeight="1">
       <c r="A160" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B160" s="2" t="inlineStr">
@@ -13018,7 +13018,7 @@
     <row r="161" ht="130" customHeight="1">
       <c r="A161" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B161" s="2" t="inlineStr">
@@ -13091,7 +13091,7 @@
     <row r="162" ht="130" customHeight="1">
       <c r="A162" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c,AU-3,AU-12 a</t>
+          <t>AU-12 c,AU-3,MA-4 (1) (a),AU-12 a</t>
         </is>
       </c>
       <c r="B162" s="2" t="inlineStr">
@@ -13164,7 +13164,7 @@
     <row r="163" ht="130" customHeight="1">
       <c r="A163" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B163" s="2" t="inlineStr">
@@ -13249,7 +13249,7 @@
     <row r="164" ht="130" customHeight="1">
       <c r="A164" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B164" s="2" t="inlineStr">
@@ -13324,7 +13324,7 @@
     <row r="165" ht="130" customHeight="1">
       <c r="A165" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B165" s="2" t="inlineStr">
@@ -13399,7 +13399,7 @@
     <row r="166" ht="130" customHeight="1">
       <c r="A166" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B166" s="2" t="inlineStr">
@@ -13474,7 +13474,7 @@
     <row r="167" ht="130" customHeight="1">
       <c r="A167" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B167" s="2" t="inlineStr">
@@ -13549,7 +13549,7 @@
     <row r="168" ht="130" customHeight="1">
       <c r="A168" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B168" s="2" t="inlineStr">
@@ -13620,7 +13620,7 @@
     <row r="169" ht="130" customHeight="1">
       <c r="A169" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B169" s="2" t="inlineStr">
@@ -13691,7 +13691,7 @@
     <row r="170" ht="130" customHeight="1">
       <c r="A170" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B170" s="2" t="inlineStr">
@@ -13763,7 +13763,7 @@
     <row r="171" ht="130" customHeight="1">
       <c r="A171" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B171" s="2" t="inlineStr">
@@ -13834,7 +13834,7 @@
     <row r="172" ht="130" customHeight="1">
       <c r="A172" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B172" s="2" t="inlineStr">
@@ -13905,7 +13905,7 @@
     <row r="173" ht="130" customHeight="1">
       <c r="A173" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B173" s="2" t="inlineStr">
@@ -13977,7 +13977,7 @@
     <row r="174" ht="130" customHeight="1">
       <c r="A174" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B174" s="2" t="inlineStr">
@@ -14052,7 +14052,7 @@
     <row r="175" ht="130" customHeight="1">
       <c r="A175" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B175" s="2" t="inlineStr">
@@ -14123,7 +14123,7 @@
     <row r="176" ht="130" customHeight="1">
       <c r="A176" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B176" s="2" t="inlineStr">
@@ -14194,7 +14194,7 @@
     <row r="177" ht="130" customHeight="1">
       <c r="A177" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-12 c</t>
+          <t>AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B177" s="2" t="inlineStr">
@@ -14266,7 +14266,7 @@
     <row r="178" ht="130" customHeight="1">
       <c r="A178" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B178" s="2" t="inlineStr">
@@ -14341,7 +14341,7 @@
     <row r="179" ht="130" customHeight="1">
       <c r="A179" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B179" s="2" t="inlineStr">
@@ -14423,7 +14423,7 @@
     <row r="180" ht="130" customHeight="1">
       <c r="A180" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B180" s="2" t="inlineStr">
@@ -14505,7 +14505,7 @@
     <row r="181" ht="130" customHeight="1">
       <c r="A181" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B181" s="2" t="inlineStr">
@@ -14587,7 +14587,7 @@
     <row r="182" ht="130" customHeight="1">
       <c r="A182" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-3</t>
+          <t>AU-3,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B182" s="2" t="inlineStr">
@@ -14669,7 +14669,7 @@
     <row r="183" ht="130" customHeight="1">
       <c r="A183" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B183" s="2" t="inlineStr">
@@ -14751,7 +14751,7 @@
     <row r="184" ht="130" customHeight="1">
       <c r="A184" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B184" s="2" t="inlineStr">
@@ -14833,7 +14833,7 @@
     <row r="185" ht="130" customHeight="1">
       <c r="A185" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B185" s="2" t="inlineStr">
@@ -14915,7 +14915,7 @@
     <row r="186" ht="130" customHeight="1">
       <c r="A186" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B186" s="2" t="inlineStr">
@@ -14997,7 +14997,7 @@
     <row r="187" ht="130" customHeight="1">
       <c r="A187" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B187" s="2" t="inlineStr">
@@ -15079,7 +15079,7 @@
     <row r="188" ht="130" customHeight="1">
       <c r="A188" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-12 c</t>
+          <t>AU-3 (1),AU-12 c,MA-4 (1) (a)</t>
         </is>
       </c>
       <c r="B188" s="2" t="inlineStr">
@@ -15157,7 +15157,7 @@
     <row r="189" ht="130" customHeight="1">
       <c r="A189" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B189" s="2" t="inlineStr">
@@ -15236,7 +15236,7 @@
     <row r="190" ht="130" customHeight="1">
       <c r="A190" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B190" s="2" t="inlineStr">
@@ -15318,7 +15318,7 @@
     <row r="191" ht="130" customHeight="1">
       <c r="A191" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B191" s="2" t="inlineStr">
@@ -15400,7 +15400,7 @@
     <row r="192" ht="130" customHeight="1">
       <c r="A192" s="2" t="inlineStr">
         <is>
-          <t>MA-4 (1) (a),AU-3 (1),AU-12 c,AU-3</t>
+          <t>AU-3,AU-12 c,MA-4 (1) (a),AU-3 (1)</t>
         </is>
       </c>
       <c r="B192" s="2" t="inlineStr">
@@ -15482,7 +15482,7 @@
     <row r="193" ht="130" customHeight="1">
       <c r="A193" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B193" s="2" t="inlineStr">
@@ -15564,7 +15564,7 @@
     <row r="194" ht="130" customHeight="1">
       <c r="A194" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,AU-12 a,MA-4 (1) (a),AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B194" s="2" t="inlineStr">
@@ -15646,7 +15646,7 @@
     <row r="195" ht="130" customHeight="1">
       <c r="A195" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B195" s="2" t="inlineStr">
@@ -15728,7 +15728,7 @@
     <row r="196" ht="130" customHeight="1">
       <c r="A196" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AU-3 (1)</t>
         </is>
       </c>
       <c r="B196" s="2" t="inlineStr">
@@ -15803,7 +15803,7 @@
     <row r="197" ht="130" customHeight="1">
       <c r="A197" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c,AU-12 a</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 a,AU-12 c,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B197" s="2" t="inlineStr">
@@ -15876,7 +15876,7 @@
     <row r="198" ht="130" customHeight="1">
       <c r="A198" s="2" t="inlineStr">
         <is>
-          <t>AU-3 (1),AC-2 (4),MA-4 (1) (a),AU-3,AU-12 c</t>
+          <t>AU-3,MA-4 (1) (a),AU-12 c,AC-2 (4),AU-3 (1)</t>
         </is>
       </c>
       <c r="B198" s="2" t="inlineStr">
@@ -15953,7 +15953,7 @@
     <row r="199" ht="130" customHeight="1">
       <c r="A199" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2 (2),IA-2 (1),IA-2 (3)</t>
+          <t>IA-2 (2),IA-2 (3),IA-2 (4),IA-2 (1)</t>
         </is>
       </c>
       <c r="B199" s="2" t="inlineStr">
@@ -16040,7 +16040,7 @@
     <row r="200" ht="130" customHeight="1">
       <c r="A200" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2,IA-2 (3),IA-2 (5),IA-2 (2)</t>
+          <t>IA-2,IA-2 (3),IA-2 (2),IA-2 (4),IA-2 (5)</t>
         </is>
       </c>
       <c r="B200" s="2" t="inlineStr">
@@ -16129,7 +16129,7 @@
     <row r="201" ht="130" customHeight="1">
       <c r="A201" s="2" t="inlineStr">
         <is>
-          <t>IA-2 (4),IA-2,IA-2 (3),IA-2 (5),IA-2 (2)</t>
+          <t>IA-2,IA-2 (3),IA-2 (2),IA-2 (4),IA-2 (5)</t>
         </is>
       </c>
       <c r="B201" s="2" t="inlineStr">
@@ -16815,7 +16815,7 @@
     <row r="210" ht="130" customHeight="1">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B210" s="2" t="inlineStr">
@@ -16892,7 +16892,7 @@
     <row r="211" ht="130" customHeight="1">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2),SC-8 (1)</t>
+          <t>SC-8 (1),SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B211" s="2" t="inlineStr">
@@ -17138,7 +17138,7 @@
     <row r="214" ht="130" customHeight="1">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>AC-11 a,SC-10</t>
+          <t>SC-10,AC-11 a</t>
         </is>
       </c>
       <c r="B214" s="2" t="inlineStr">
@@ -17906,7 +17906,7 @@
     <row r="224" ht="130" customHeight="1">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-12 a</t>
+          <t>AU-12 a,CM-6 b</t>
         </is>
       </c>
       <c r="B224" s="2" t="inlineStr">
@@ -17992,7 +17992,7 @@
     <row r="225" ht="130" customHeight="1">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-5 (2),SC-5</t>
+          <t>SC-5 (2),CM-6 b,SC-5</t>
         </is>
       </c>
       <c r="B225" s="2" t="inlineStr">
@@ -18264,7 +18264,7 @@
     <row r="228" ht="130" customHeight="1">
       <c r="A228" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16</t>
+          <t>SI-16,CM-6 b</t>
         </is>
       </c>
       <c r="B228" s="2" t="inlineStr">
@@ -18362,7 +18362,7 @@
     <row r="229" ht="130" customHeight="1">
       <c r="A229" s="2" t="inlineStr">
         <is>
-          <t>IA-8,IA-2,AU-3 (1)</t>
+          <t>IA-2,IA-8,AU-3 (1)</t>
         </is>
       </c>
       <c r="B229" s="2" t="inlineStr">
@@ -19336,7 +19336,7 @@
     <row r="241" ht="130" customHeight="1">
       <c r="A241" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-16,SC-2</t>
+          <t>SI-16,CM-6 b,SC-2</t>
         </is>
       </c>
       <c r="B241" s="2" t="inlineStr">
@@ -19496,7 +19496,7 @@
     <row r="243" ht="130" customHeight="1">
       <c r="A243" s="2" t="inlineStr">
         <is>
-          <t>SI-16,SC-3</t>
+          <t>SC-3,SI-16</t>
         </is>
       </c>
       <c r="B243" s="2" t="inlineStr">
@@ -19658,7 +19658,7 @@
     <row r="245" ht="130" customHeight="1">
       <c r="A245" s="2" t="inlineStr">
         <is>
-          <t>AC-18 (1),CM-7 a</t>
+          <t>CM-7 a,AC-18 (1)</t>
         </is>
       </c>
       <c r="B245" s="2" t="inlineStr">
@@ -20194,7 +20194,7 @@
     <row r="252" ht="130" customHeight="1">
       <c r="A252" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-5 (1) (b),IA-5 (1) (a)</t>
+          <t>IA-5 (1) (b),CM-6 b,IA-5 (1) (a)</t>
         </is>
       </c>
       <c r="B252" s="2" t="inlineStr">
@@ -20254,7 +20254,7 @@
           <t>To verify if root user is required to use complex passwords, run the following command:
  $ grep enforce_for_root /etc/security/pwquality.conf 
 The output should return "enforce_for_root" uncommented.
-If enforce_for_root is not uncommented or configured correctly then this is a finding.</t>
+If enforce_for_root is commented or not configured correctly then this is a finding.</t>
         </is>
       </c>
       <c r="L252" s="2" t="n"/>
@@ -21514,7 +21514,7 @@
     <row r="268" ht="130" customHeight="1">
       <c r="A268" s="2" t="inlineStr">
         <is>
-          <t>CM-5 (1),AU-12 (3),AU-8 b,AU-7 a,AC-6 (8),AU-7 b,AC-6 (9)</t>
+          <t>AC-6 (9),AC-6 (8),CM-5 (1),AU-7 b,AU-8 b,AU-7 a,AU-12 (3)</t>
         </is>
       </c>
       <c r="B268" s="2" t="inlineStr">
@@ -22108,7 +22108,7 @@
     <row r="276" ht="130" customHeight="1">
       <c r="A276" s="2" t="inlineStr">
         <is>
-          <t>AU-9,AU-12 c</t>
+          <t>AU-12 c,AU-9</t>
         </is>
       </c>
       <c r="B276" s="2" t="inlineStr">
@@ -24145,7 +24145,7 @@
     <row r="302" ht="130" customHeight="1">
       <c r="A302" s="2" t="inlineStr">
         <is>
-          <t>AC-6 (9),AU-12 c,AC-2 (4)</t>
+          <t>AC-2 (4),AU-12 c,AC-6 (9)</t>
         </is>
       </c>
       <c r="B302" s="2" t="inlineStr">
@@ -27874,7 +27874,7 @@
     <row r="351" ht="130" customHeight="1">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-2 (2)</t>
+          <t>IA-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B351" s="2" t="inlineStr">
@@ -27954,7 +27954,7 @@
     <row r="352" ht="130" customHeight="1">
       <c r="A352" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B352" s="2" t="inlineStr">
@@ -28027,7 +28027,7 @@
     <row r="353" ht="130" customHeight="1">
       <c r="A353" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,CM-5 (1)</t>
+          <t>CM-5 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B353" s="2" t="inlineStr">
@@ -28607,7 +28607,7 @@
     <row r="361" ht="130" customHeight="1">
       <c r="A361" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AC-17 (2)</t>
+          <t>AC-17 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B361" s="2" t="inlineStr">
@@ -30335,7 +30335,7 @@
     <row r="384" ht="130" customHeight="1">
       <c r="A384" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,AU-3</t>
+          <t>AU-3,CM-6 b</t>
         </is>
       </c>
       <c r="B384" s="2" t="inlineStr">
@@ -30579,7 +30579,7 @@
     <row r="387" ht="130" customHeight="1">
       <c r="A387" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B387" s="2" t="inlineStr">
@@ -30973,7 +30973,7 @@
     <row r="392" ht="130" customHeight="1">
       <c r="A392" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),AC-17 (9),CM-6 b,CM-7 b</t>
+          <t>CM-7 b,AC-17 (9),AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B392" s="2" t="inlineStr">
@@ -31051,7 +31051,7 @@
     <row r="393" ht="130" customHeight="1">
       <c r="A393" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-6 b,CM-7 b</t>
+          <t>CM-7 b,AC-17 (1),CM-6 b</t>
         </is>
       </c>
       <c r="B393" s="2" t="inlineStr">
@@ -33550,7 +33550,7 @@
     <row r="422" ht="130" customHeight="1">
       <c r="A422" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B422" s="2" t="inlineStr">
@@ -33625,7 +33625,7 @@
     <row r="423" ht="130" customHeight="1">
       <c r="A423" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B423" s="2" t="inlineStr">
@@ -34312,7 +34312,7 @@
     <row r="432" ht="130" customHeight="1">
       <c r="A432" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B432" s="2" t="inlineStr">
@@ -34915,7 +34915,7 @@
     <row r="439" ht="130" customHeight="1">
       <c r="A439" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SC-3</t>
+          <t>SC-3,CM-6 b</t>
         </is>
       </c>
       <c r="B439" s="2" t="inlineStr">
@@ -35367,7 +35367,7 @@
     <row r="445" ht="130" customHeight="1">
       <c r="A445" s="2" t="inlineStr">
         <is>
-          <t>AU-4,CM-6 b</t>
+          <t>CM-6 b,AU-4</t>
         </is>
       </c>
       <c r="B445" s="2" t="inlineStr">
@@ -35667,7 +35667,7 @@
     <row r="449" ht="130" customHeight="1">
       <c r="A449" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B449" s="2" t="inlineStr">
@@ -35744,7 +35744,7 @@
     <row r="450" ht="130" customHeight="1">
       <c r="A450" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,IA-3</t>
+          <t>IA-3,CM-6 b</t>
         </is>
       </c>
       <c r="B450" s="2" t="inlineStr">
@@ -36126,7 +36126,7 @@
     <row r="455" ht="130" customHeight="1">
       <c r="A455" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B455" s="2" t="inlineStr">
@@ -36773,7 +36773,7 @@
     <row r="464" ht="130" customHeight="1">
       <c r="A464" s="2" t="inlineStr">
         <is>
-          <t>CM-6 b,SI-2 (2)</t>
+          <t>SI-2 (2),CM-6 b</t>
         </is>
       </c>
       <c r="B464" s="2" t="inlineStr">
@@ -37064,7 +37064,7 @@
     <row r="468" ht="130" customHeight="1">
       <c r="A468" s="2" t="inlineStr">
         <is>
-          <t>AC-12,MA-4 e,MA-4 (7),SC-10</t>
+          <t>MA-4 (7),AC-12,SC-10,MA-4 e</t>
         </is>
       </c>
       <c r="B468" s="2" t="inlineStr">
@@ -37294,7 +37294,7 @@
     <row r="471" ht="130" customHeight="1">
       <c r="A471" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B471" s="2" t="inlineStr">
@@ -38589,7 +38589,7 @@
     <row r="488" ht="130" customHeight="1">
       <c r="A488" s="2" t="inlineStr">
         <is>
-          <t>IA-3,CM-7 b</t>
+          <t>CM-7 b,IA-3</t>
         </is>
       </c>
       <c r="B488" s="2" t="inlineStr">
@@ -38879,7 +38879,7 @@
     <row r="492" ht="130" customHeight="1">
       <c r="A492" s="2" t="inlineStr">
         <is>
-          <t>AC-17 (1),CM-7 b</t>
+          <t>CM-7 b,AC-17 (1)</t>
         </is>
       </c>
       <c r="B492" s="2" t="inlineStr">
@@ -39896,7 +39896,7 @@
     <row r="505" ht="130" customHeight="1">
       <c r="A505" s="2" t="inlineStr">
         <is>
-          <t>AU-4,AU-4 (1)</t>
+          <t>AU-4 (1),AU-4</t>
         </is>
       </c>
       <c r="B505" s="2" t="inlineStr">
@@ -40135,7 +40135,7 @@
     <row r="508" ht="130" customHeight="1">
       <c r="A508" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B508" s="2" t="inlineStr">
@@ -40237,7 +40237,7 @@
     <row r="509" ht="130" customHeight="1">
       <c r="A509" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B509" s="2" t="inlineStr">
@@ -40347,7 +40347,7 @@
     <row r="510" ht="130" customHeight="1">
       <c r="A510" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B510" s="2" t="inlineStr">
@@ -40458,7 +40458,7 @@
     <row r="511" ht="130" customHeight="1">
       <c r="A511" s="2" t="inlineStr">
         <is>
-          <t>AC-8 a,AC-8 c 1, AC-8 c 2, AC-8 c 3</t>
+          <t>AC-8 c 1, AC-8 c 2, AC-8 c 3,AC-8 a</t>
         </is>
       </c>
       <c r="B511" s="2" t="inlineStr">
@@ -40930,7 +40930,7 @@
 attacks.
 Password complexity is one factor of several that determines how long it takes
 to crack a password. The more complex the password, the greater the number of
-possble combinations that need to be tested before the password is compromised.
+possible combinations that need to be tested before the password is compromised.
 Requiring a minimum number of special characters makes password guessing attacks
 more difficult by ensuring a larger search space.</t>
         </is>
@@ -40949,14 +40949,21 @@
         <is>
           <t>To check how many special characters are required in a password, run the following command:
  $ grep ocredit /etc/security/pwquality.conf 
-The "ocredit" parameter (as a negative number) will indicate how many special characters are required.
+The "ocredit" parameter (as a negative number) will indicate how many special
+characters are required.
 The DoD and FISMA require at least one special character in a password.
 This would appear as "ocredit = -1".
-If ocredit is not found or not equal to or less than the required value then this is a finding.</t>
+If value of "ocredit" is a positive number or is commented out then this is a finding.</t>
         </is>
       </c>
       <c r="L516" s="2" t="n"/>
-      <c r="M516" s="2" t="inlineStr"/>
+      <c r="M516" s="2" t="inlineStr">
+        <is>
+          <t>Add or modify the "ocredit" option line in /etc/security/pwquality.conf to have the required
+value, like in the following example:
+ocredit = 1</t>
+        </is>
+      </c>
       <c r="N516" s="2" t="inlineStr">
         <is>
           <t>CAT II</t>
@@ -41161,7 +41168,7 @@
     <row r="520" ht="130" customHeight="1">
       <c r="A520" s="2" t="inlineStr">
         <is>
-          <t>SC-8,SC-8 (2)</t>
+          <t>SC-8 (2),SC-8</t>
         </is>
       </c>
       <c r="B520" s="2" t="inlineStr">
@@ -42274,7 +42281,7 @@
     <row r="534" ht="130" customHeight="1">
       <c r="A534" s="2" t="inlineStr">
         <is>
-          <t>SC-8,AC-17 (2)</t>
+          <t>AC-17 (2),SC-8</t>
         </is>
       </c>
       <c r="B534" s="2" t="inlineStr">

</xml_diff>